<commit_message>
BP-644 geocord fixed, educationalInterval patched
</commit_message>
<xml_diff>
--- a/assets/extData.xlsx
+++ b/assets/extData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3090" uniqueCount="1346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3109" uniqueCount="1364">
   <si>
     <t>Полное название</t>
   </si>
@@ -1822,13 +1822,13 @@
 Центральный административный округ</t>
   </si>
   <si>
-    <t>Басманный район
-Басманный район
+    <t>Басманный район;
+Басманный район;
 Тверской район</t>
   </si>
   <si>
-    <t>Большой Харитоньевский переулок
-Лялин переулок, д. 3А
+    <t>Большой Харитоньевский переулок;
+Лялин переулок, д. 3А;
 3-й Колобовский переулок</t>
   </si>
   <si>
@@ -5525,7 +5525,7 @@
 10</t>
   </si>
   <si>
-    <t>Лицей с кружками по флэш-анимации, системному программированию и робототехнике</t>
+    <t>Лицей с занятиями по флэш-анимации, системному программированию и робототехнике</t>
   </si>
   <si>
     <t xml:space="preserve">ассоциированная школа ЮНЕСКО; Сотрудничает с Microsoft, ABBY,  1C и Лабораторией Касперского; сотрудничает с факультетом ВМК МГУ, РГУ нефти и газа имени И.М.Губкина; </t>
@@ -5666,6 +5666,9 @@
     <t xml:space="preserve">Государственное бюджетное общеобразовательное учреждение города Москвы "Гимназия № 1358" </t>
   </si>
   <si>
+    <t>Гимназия №1358</t>
+  </si>
+  <si>
     <t>http://gym1358sz.mskobr.ru/</t>
   </si>
   <si>
@@ -5673,6 +5676,18 @@
 </t>
   </si>
   <si>
+    <t>20802 (школа №1549)
+102490 (школа №1358)
+20801 (школа №1192)</t>
+  </si>
+  <si>
+    <t>социально-экономический; социально-гуманитарный; физико-математический; биолого-химический; филологический
+10</t>
+  </si>
+  <si>
+    <t>победитель второго этапа проекта  "Школа Новых Технологий"; Лауреат Гранта Мэра Москвы в сфере образования; социально-гуманитарный профиль при поддержке МФПУ "Синергия"; в школе действует три отделения: общеобразовательное, гимназическое, с углубленным изучением иностранных языков</t>
+  </si>
+  <si>
     <t>2000 р/мес</t>
   </si>
   <si>
@@ -5706,7 +5721,56 @@
     <t>Государственное бюджетное общеобразовательное учреждение города Москвы "Школа с углубленным изучением французского языка № 1251 имени генерала Шарля де Голля"</t>
   </si>
   <si>
+    <t>http://sch1251s.mskobr.ru/</t>
+  </si>
+  <si>
+    <t>https://vk.com/club916655 - Школа № 1251 имени генерала Шарля де Голля
+</t>
+  </si>
+  <si>
+    <t>углубленное изучение французского языка
+1
+физико-математический; технологический; гуманитарный; социально-гуманитарный; социальный; универсальный
+10</t>
+  </si>
+  <si>
+    <t>ополнительное бесплатное языковое образование по французскому языку 
+сотрудничает с МГУ, МГПУ, НИУ ВШЭ и МГОУ
+ассоциированная школа ЮНЕСКО</t>
+  </si>
+  <si>
+    <t>не предусмотрено</t>
+  </si>
+  <si>
     <t>Государственное бюджетное общеобразовательное учреждение города Москвы "Школа № 1434 "Раменки"</t>
+  </si>
+  <si>
+    <t>Школа № 1434 "Раменки"</t>
+  </si>
+  <si>
+    <t>http://sch1434.mskobr.ru/</t>
+  </si>
+  <si>
+    <t>https://vk.com/school.active - Актив школы 1434
+</t>
+  </si>
+  <si>
+    <t>457541
+1151 (школа №1119)</t>
+  </si>
+  <si>
+    <t>филологический; физико-математический; химико-биологический
+10</t>
+  </si>
+  <si>
+    <t>Школа с программой Международного бакалвариата,  кадетскими классами и своей лингвистической школой</t>
+  </si>
+  <si>
+    <t>4000 р/мес</t>
+  </si>
+  <si>
+    <t>https://vk.com/club6074 - Выпускники школы 1134 и выпускники ЦО 1434. г.М
+</t>
   </si>
   <si>
     <t>Твоё название</t>
@@ -5722,9 +5786,6 @@
   <si>
     <t>был открыт  как экспериментальный лицей с востоковедным уклоном  при ИСАА МГУ в 1991 году;  с 2011 по 2015 крепко удерживает лидерство среди московских школ;реализует программу Дополнительного образования для школьников 13-18 лет,где ведется подготовка к олимпиадам; при лицее работает «Открытая школа»; ежегодно летом  две естественнонаучные экспедиции выезжают  на Белое море и на озеро Байкал;
 </t>
-  </si>
-  <si>
-    <t>не предусмотрено</t>
   </si>
   <si>
     <t>физико-математической (включая компьютерно-информационный класс); химический; биологический.
@@ -5883,6 +5944,16 @@
   </si>
   <si>
     <t xml:space="preserve">не предусмотрено </t>
+  </si>
+  <si>
+    <t>Басманный район
+Басманный район
+Тверской район</t>
+  </si>
+  <si>
+    <t>Большой Харитоньевский переулок
+Лялин переулок, д. 3А
+3-й Колобовский переулок</t>
   </si>
   <si>
     <t>физико-математический; гуманитарный
@@ -6438,7 +6509,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -6509,6 +6580,9 @@
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
@@ -12590,7 +12664,7 @@
         <v>1109</v>
       </c>
       <c r="J204" s="1" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="K204" s="1" t="s">
         <v>26</v>
@@ -13094,20 +13168,26 @@
         <v>1176</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>836</v>
+        <v>1177</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>1178</v>
-      </c>
-      <c r="E226" s="6"/>
-      <c r="F226" s="6"/>
+        <v>1179</v>
+      </c>
+      <c r="E226" s="1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>1181</v>
+      </c>
       <c r="G226" s="6"/>
-      <c r="H226" s="6"/>
+      <c r="H226" s="1" t="s">
+        <v>1182</v>
+      </c>
       <c r="I226" s="1" t="s">
-        <v>1179</v>
+        <v>1183</v>
       </c>
       <c r="J226" s="1" t="s">
         <v>44</v>
@@ -13135,11 +13215,11 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="s">
-        <v>1180</v>
+        <v>1184</v>
       </c>
       <c r="B228" s="6"/>
       <c r="C228" s="4" t="s">
-        <v>1181</v>
+        <v>1185</v>
       </c>
       <c r="D228" s="6"/>
       <c r="E228" s="6"/>
@@ -13167,7 +13247,7 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="s">
-        <v>1182</v>
+        <v>1186</v>
       </c>
       <c r="B230" s="6"/>
       <c r="C230" s="6"/>
@@ -13197,7 +13277,7 @@
     </row>
     <row r="232">
       <c r="A232" s="1" t="s">
-        <v>1183</v>
+        <v>1187</v>
       </c>
       <c r="B232" s="6"/>
       <c r="C232" s="6"/>
@@ -13213,7 +13293,7 @@
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
-        <v>1184</v>
+        <v>1188</v>
       </c>
       <c r="B233" s="6"/>
       <c r="C233" s="6"/>
@@ -13229,7 +13309,7 @@
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
-        <v>1185</v>
+        <v>1189</v>
       </c>
       <c r="B234" s="6"/>
       <c r="C234" s="6"/>
@@ -13259,7 +13339,7 @@
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
-        <v>1186</v>
+        <v>1190</v>
       </c>
       <c r="B236" s="6"/>
       <c r="C236" s="6"/>
@@ -13275,7 +13355,7 @@
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
-        <v>1187</v>
+        <v>1191</v>
       </c>
       <c r="B237" s="6"/>
       <c r="C237" s="6"/>
@@ -13291,7 +13371,7 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>1188</v>
+        <v>1192</v>
       </c>
       <c r="B238" s="6"/>
       <c r="C238" s="6"/>
@@ -13307,51 +13387,85 @@
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
-        <v>1189</v>
+        <v>1193</v>
       </c>
       <c r="B239" s="6"/>
-      <c r="C239" s="6"/>
-      <c r="D239" s="6"/>
-      <c r="E239" s="6"/>
-      <c r="F239" s="6"/>
+      <c r="C239" s="4" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D239" s="1" t="s">
+        <v>1195</v>
+      </c>
+      <c r="E239" s="1">
+        <v>2510.0</v>
+      </c>
+      <c r="F239" s="1" t="s">
+        <v>1196</v>
+      </c>
       <c r="G239" s="6"/>
-      <c r="H239" s="6"/>
+      <c r="H239" s="1" t="s">
+        <v>1197</v>
+      </c>
       <c r="I239" s="6"/>
       <c r="J239" s="6"/>
-      <c r="K239" s="6"/>
-      <c r="L239" s="6"/>
+      <c r="K239" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L239" s="1" t="s">
+        <v>1198</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>1190</v>
-      </c>
-      <c r="B240" s="6"/>
-      <c r="C240" s="6"/>
-      <c r="D240" s="6"/>
-      <c r="E240" s="6"/>
-      <c r="F240" s="6"/>
-      <c r="G240" s="6"/>
-      <c r="H240" s="6"/>
-      <c r="I240" s="6"/>
-      <c r="J240" s="6"/>
-      <c r="K240" s="6"/>
-      <c r="L240" s="6"/>
+        <v>1199</v>
+      </c>
+      <c r="B240" s="1" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C240" s="4" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D240" s="1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E240" s="1" t="s">
+        <v>1203</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G240" s="1" t="s">
+        <v>1205</v>
+      </c>
+      <c r="H240" s="24"/>
+      <c r="I240" s="1" t="s">
+        <v>1206</v>
+      </c>
+      <c r="J240" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K240" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L240" s="1" t="s">
+        <v>1198</v>
+      </c>
     </row>
     <row r="241">
-      <c r="A241" s="7" t="s">
-        <v>1102</v>
-      </c>
-      <c r="B241" s="8"/>
-      <c r="C241" s="8"/>
-      <c r="D241" s="8"/>
-      <c r="E241" s="8"/>
-      <c r="F241" s="8"/>
-      <c r="G241" s="8"/>
+      <c r="A241" s="7"/>
+      <c r="B241" s="7"/>
+      <c r="C241" s="7"/>
+      <c r="D241" s="7" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E241" s="7"/>
+      <c r="F241" s="7"/>
+      <c r="G241" s="7"/>
       <c r="H241" s="8"/>
-      <c r="I241" s="8"/>
-      <c r="J241" s="8"/>
-      <c r="K241" s="8"/>
-      <c r="L241" s="8"/>
+      <c r="I241" s="7"/>
+      <c r="J241" s="7"/>
+      <c r="K241" s="7"/>
+      <c r="L241" s="7"/>
       <c r="M241" s="9"/>
       <c r="N241" s="9"/>
       <c r="O241" s="9"/>
@@ -25285,8 +25399,10 @@
     <hyperlink r:id="rId164" ref="C224"/>
     <hyperlink r:id="rId165" ref="C226"/>
     <hyperlink r:id="rId166" ref="C228"/>
+    <hyperlink r:id="rId167" ref="C239"/>
+    <hyperlink r:id="rId168" ref="C240"/>
   </hyperlinks>
-  <drawing r:id="rId167"/>
+  <drawing r:id="rId169"/>
 </worksheet>
 </file>
 
@@ -25320,7 +25436,7 @@
         <v>1.0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1191</v>
+        <v>1208</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -25330,7 +25446,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1192</v>
+        <v>1209</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -25389,7 +25505,7 @@
         <v>4474.0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1193</v>
+        <v>1210</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>22</v>
@@ -25398,10 +25514,10 @@
         <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>1194</v>
+        <v>1211</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>25</v>
@@ -25410,7 +25526,7 @@
         <v>26</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>27</v>
@@ -25502,10 +25618,10 @@
         <v>48659.0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1196</v>
+        <v>1212</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1197</v>
+        <v>1213</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>41</v>
@@ -25514,7 +25630,7 @@
         <v>42</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>25</v>
@@ -25612,7 +25728,7 @@
         <v>1378.0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1198</v>
+        <v>1214</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>57</v>
@@ -25621,7 +25737,7 @@
         <v>58</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>1199</v>
+        <v>1215</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>60</v>
@@ -25633,7 +25749,7 @@
         <v>61</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>62</v>
@@ -25686,10 +25802,10 @@
       <c r="E10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="24" t="s">
-        <v>1200</v>
-      </c>
-      <c r="G10" s="24" t="s">
+      <c r="F10" s="25" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G10" s="25" t="s">
         <v>74</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -25699,7 +25815,7 @@
         <v>76</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>44</v>
@@ -25708,7 +25824,7 @@
         <v>26</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>1201</v>
+        <v>1217</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>77</v>
@@ -25780,7 +25896,7 @@
         <v>53301.0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1202</v>
+        <v>1218</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>89</v>
@@ -25789,10 +25905,10 @@
         <v>90</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>1203</v>
+        <v>1219</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>44</v>
@@ -25801,7 +25917,7 @@
         <v>26</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>92</v>
@@ -25875,7 +25991,7 @@
         <v>26682.0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1204</v>
+        <v>1220</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>105</v>
@@ -25887,7 +26003,7 @@
         <v>107</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>25</v>
@@ -25968,7 +26084,7 @@
         <v>4873.0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1205</v>
+        <v>1221</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>120</v>
@@ -25980,7 +26096,7 @@
         <v>122</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>44</v>
@@ -25989,7 +26105,7 @@
         <v>43</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>123</v>
@@ -26061,7 +26177,7 @@
         <v>135</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1206</v>
+        <v>1222</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>136</v>
@@ -26073,7 +26189,7 @@
         <v>138</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>44</v>
@@ -26082,7 +26198,7 @@
         <v>26</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>139</v>
@@ -26137,10 +26253,10 @@
         <v>189133.0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>1207</v>
+        <v>1223</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>1208</v>
+        <v>1224</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>151</v>
@@ -26158,7 +26274,7 @@
         <v>61</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>154</v>
@@ -26215,7 +26331,7 @@
         <v>166</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>1209</v>
+        <v>1225</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>167</v>
@@ -26236,7 +26352,7 @@
         <v>26</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>172</v>
@@ -26248,7 +26364,7 @@
         <v>174</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>1210</v>
+        <v>1226</v>
       </c>
       <c r="R26" s="2" t="s">
         <v>176</v>
@@ -26289,7 +26405,7 @@
         <v>182</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1211</v>
+        <v>1227</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>183</v>
@@ -26310,7 +26426,7 @@
         <v>26</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>187</v>
@@ -26384,7 +26500,7 @@
         <v>946.0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>1212</v>
+        <v>1228</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>201</v>
@@ -26396,7 +26512,7 @@
         <v>203</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>25</v>
@@ -26405,7 +26521,7 @@
         <v>204</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N31" s="2" t="s">
         <v>45</v>
@@ -26517,7 +26633,7 @@
         <v>802.0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1213</v>
+        <v>1229</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>220</v>
@@ -26538,7 +26654,7 @@
         <v>204</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>92</v>
@@ -26613,7 +26729,7 @@
         <v>235</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>1214</v>
+        <v>1230</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>236</v>
@@ -26634,7 +26750,7 @@
         <v>26</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N39" s="2" t="s">
         <v>240</v>
@@ -26708,7 +26824,7 @@
         <v>589.0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>1215</v>
+        <v>1231</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>253</v>
@@ -26717,7 +26833,7 @@
         <v>254</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>1216</v>
+        <v>1232</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>60</v>
@@ -26729,7 +26845,7 @@
         <v>43</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N42" s="2" t="s">
         <v>256</v>
@@ -26805,10 +26921,10 @@
         <v>12904.0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>1217</v>
+        <v>1233</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1218</v>
+        <v>1234</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>271</v>
@@ -26826,7 +26942,7 @@
         <v>61</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>275</v>
@@ -26960,7 +27076,7 @@
         <v>289</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>1219</v>
+        <v>1235</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>290</v>
@@ -26972,7 +27088,7 @@
         <v>292</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>1220</v>
+        <v>1236</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>294</v>
@@ -26981,7 +27097,7 @@
         <v>43</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>295</v>
@@ -27070,7 +27186,7 @@
         <v>308</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>1221</v>
+        <v>1237</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>309</v>
@@ -27091,7 +27207,7 @@
         <v>26</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N56" s="2" t="s">
         <v>313</v>
@@ -27163,7 +27279,7 @@
         <v>1909.0</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>1222</v>
+        <v>1238</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>325</v>
@@ -27175,7 +27291,7 @@
         <v>327</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>328</v>
@@ -27184,7 +27300,7 @@
         <v>43</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>329</v>
@@ -27239,10 +27355,10 @@
         <v>339</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>1223</v>
+        <v>1239</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1224</v>
+        <v>1240</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>341</v>
@@ -27260,7 +27376,7 @@
         <v>43</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N61" s="2" t="s">
         <v>344</v>
@@ -27334,7 +27450,7 @@
         <v>357</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>1225</v>
+        <v>1241</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>358</v>
@@ -27343,10 +27459,10 @@
         <v>359</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>1226</v>
+        <v>1242</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>25</v>
@@ -27355,7 +27471,7 @@
         <v>26</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N64" s="2" t="s">
         <v>361</v>
@@ -27393,7 +27509,7 @@
         <v>371</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>1227</v>
+        <v>1243</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>372</v>
@@ -27405,7 +27521,7 @@
         <v>374</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>25</v>
@@ -27414,7 +27530,7 @@
         <v>26</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N65" s="14" t="s">
         <v>375</v>
@@ -27484,7 +27600,7 @@
         <v>386</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>1228</v>
+        <v>1244</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>387</v>
@@ -27493,10 +27609,10 @@
         <v>388</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>1229</v>
+        <v>1245</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>1230</v>
+        <v>1246</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>44</v>
@@ -27505,7 +27621,7 @@
         <v>26</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N68" s="2" t="s">
         <v>391</v>
@@ -27558,7 +27674,7 @@
         <v>1724839.0</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>1231</v>
+        <v>1247</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>401</v>
@@ -27570,7 +27686,7 @@
         <v>403</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>1232</v>
+        <v>1248</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>25</v>
@@ -27579,16 +27695,16 @@
         <v>26</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N70" s="2" t="s">
         <v>404</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>405</v>
+        <v>1249</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>406</v>
+        <v>1250</v>
       </c>
       <c r="Q70" s="2" t="s">
         <v>407</v>
@@ -27634,7 +27750,7 @@
         <v>47525.0</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>1233</v>
+        <v>1251</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>415</v>
@@ -27655,7 +27771,7 @@
         <v>43</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N72" s="2" t="s">
         <v>419</v>
@@ -27729,10 +27845,10 @@
         <v>779.0</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>1234</v>
+        <v>1252</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>1235</v>
+        <v>1253</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>433</v>
@@ -27750,7 +27866,7 @@
         <v>61</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N75" s="2" t="s">
         <v>436</v>
@@ -27805,10 +27921,10 @@
         <v>3671.0</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1236</v>
+        <v>1254</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>1237</v>
+        <v>1255</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>448</v>
@@ -27817,7 +27933,7 @@
         <v>449</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>44</v>
@@ -27826,7 +27942,7 @@
         <v>204</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N77" s="2" t="s">
         <v>450</v>
@@ -27879,7 +27995,7 @@
         <v>460</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>1238</v>
+        <v>1256</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>461</v>
@@ -27900,7 +28016,7 @@
         <v>43</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N79" s="2" t="s">
         <v>465</v>
@@ -27972,16 +28088,16 @@
         <v>766.0</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>1239</v>
+        <v>1257</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>1240</v>
+        <v>1258</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>478</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>1241</v>
+        <v>1259</v>
       </c>
       <c r="J82" s="1" t="s">
         <v>480</v>
@@ -27993,7 +28109,7 @@
         <v>43</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N82" s="2" t="s">
         <v>481</v>
@@ -28065,16 +28181,16 @@
         <v>493</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>1242</v>
+        <v>1260</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>1243</v>
+        <v>1261</v>
       </c>
       <c r="H85" s="2" t="s">
         <v>495</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>1244</v>
+        <v>1262</v>
       </c>
       <c r="J85" s="1" t="s">
         <v>497</v>
@@ -28086,7 +28202,7 @@
         <v>498</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N85" s="2" t="s">
         <v>499</v>
@@ -28139,7 +28255,7 @@
         <v>8229.0</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>1245</v>
+        <v>1263</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>509</v>
@@ -28148,7 +28264,7 @@
         <v>510</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>1246</v>
+        <v>1264</v>
       </c>
       <c r="J87" s="1" t="s">
         <v>512</v>
@@ -28160,7 +28276,7 @@
         <v>513</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N87" s="2" t="s">
         <v>514</v>
@@ -28198,7 +28314,7 @@
         <v>1590.0</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>1247</v>
+        <v>1265</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>524</v>
@@ -28219,7 +28335,7 @@
         <v>204</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N88" s="2" t="s">
         <v>528</v>
@@ -28274,16 +28390,16 @@
         <v>540</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>1248</v>
+        <v>1266</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>1249</v>
+        <v>1267</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>542</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>1250</v>
+        <v>1268</v>
       </c>
       <c r="J90" s="2" t="s">
         <v>544</v>
@@ -28295,7 +28411,7 @@
         <v>43</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N90" s="2" t="s">
         <v>545</v>
@@ -28369,13 +28485,13 @@
         <v>1228.0</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>1251</v>
+        <v>1269</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>558</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>1252</v>
+        <v>1270</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>560</v>
@@ -28390,7 +28506,7 @@
         <v>204</v>
       </c>
       <c r="M93" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N93" s="2" t="s">
         <v>562</v>
@@ -28446,16 +28562,16 @@
         <v>9883.0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>1253</v>
+        <v>1271</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>574</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>1254</v>
+        <v>1272</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>1255</v>
+        <v>1273</v>
       </c>
       <c r="J95" s="1" t="s">
         <v>577</v>
@@ -28467,7 +28583,7 @@
         <v>43</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N95" s="2" t="s">
         <v>578</v>
@@ -28536,7 +28652,7 @@
         <v>420.0</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>1256</v>
+        <v>1274</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>589</v>
@@ -28545,7 +28661,7 @@
         <v>590</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>1257</v>
+        <v>1275</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>60</v>
@@ -28557,7 +28673,7 @@
         <v>43</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N98" s="2" t="s">
         <v>592</v>
@@ -28612,7 +28728,7 @@
         <v>1927.0</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>1258</v>
+        <v>1276</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>603</v>
@@ -28633,7 +28749,7 @@
         <v>204</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N100" s="2" t="s">
         <v>606</v>
@@ -28705,7 +28821,7 @@
         <v>2303.0</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>1259</v>
+        <v>1277</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>618</v>
@@ -28726,7 +28842,7 @@
         <v>43</v>
       </c>
       <c r="M103" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N103" s="2" t="s">
         <v>436</v>
@@ -28764,7 +28880,7 @@
         <v>8813.0</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>1260</v>
+        <v>1278</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>631</v>
@@ -28785,7 +28901,7 @@
         <v>43</v>
       </c>
       <c r="M104" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N104" s="2" t="s">
         <v>635</v>
@@ -28823,10 +28939,10 @@
         <v>55505.0</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>1261</v>
+        <v>1279</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>1262</v>
+        <v>1280</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>646</v>
@@ -28844,7 +28960,7 @@
         <v>204</v>
       </c>
       <c r="M105" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N105" s="2" t="s">
         <v>648</v>
@@ -28890,7 +29006,7 @@
         <v>656</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>1263</v>
+        <v>1281</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>657</v>
@@ -28911,7 +29027,7 @@
         <v>204</v>
       </c>
       <c r="M107" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N107" s="2" t="s">
         <v>660</v>
@@ -28957,7 +29073,7 @@
         <v>4044.0</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>1264</v>
+        <v>1282</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>668</v>
@@ -28966,7 +29082,7 @@
         <v>669</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>1265</v>
+        <v>1283</v>
       </c>
       <c r="J109" s="1" t="s">
         <v>561</v>
@@ -28978,7 +29094,7 @@
         <v>204</v>
       </c>
       <c r="M109" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N109" s="2" t="s">
         <v>671</v>
@@ -29022,13 +29138,13 @@
         <v>678</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>1266</v>
+        <v>1284</v>
       </c>
       <c r="G111" s="1" t="s">
         <v>679</v>
       </c>
       <c r="H111" s="14" t="s">
-        <v>1267</v>
+        <v>1285</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>681</v>
@@ -29043,7 +29159,7 @@
         <v>43</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N111" s="2" t="s">
         <v>683</v>
@@ -29089,13 +29205,13 @@
         <v>58288.0</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>1268</v>
+        <v>1286</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>691</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>1269</v>
+        <v>1287</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>693</v>
@@ -29110,7 +29226,7 @@
         <v>26</v>
       </c>
       <c r="M113" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N113" s="2" t="s">
         <v>606</v>
@@ -29154,13 +29270,13 @@
         <v>701</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>1270</v>
+        <v>1288</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>702</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>1271</v>
+        <v>1289</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>704</v>
@@ -29175,7 +29291,7 @@
         <v>43</v>
       </c>
       <c r="M115" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N115" s="2" t="s">
         <v>706</v>
@@ -29221,7 +29337,7 @@
         <v>714</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>1272</v>
+        <v>1290</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>715</v>
@@ -29242,7 +29358,7 @@
         <v>43</v>
       </c>
       <c r="M117" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N117" s="2" t="s">
         <v>719</v>
@@ -29286,7 +29402,7 @@
         <v>9295.0</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>1273</v>
+        <v>1291</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>726</v>
@@ -29298,7 +29414,7 @@
         <v>728</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>25</v>
@@ -29307,7 +29423,7 @@
         <v>26</v>
       </c>
       <c r="M119" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N119" s="2" t="s">
         <v>729</v>
@@ -29353,7 +29469,7 @@
         <v>78380.0</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>1274</v>
+        <v>1292</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>737</v>
@@ -29374,7 +29490,7 @@
         <v>61</v>
       </c>
       <c r="M121" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N121" s="2" t="s">
         <v>740</v>
@@ -29420,7 +29536,7 @@
         <v>1738982.0</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>1275</v>
+        <v>1293</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>748</v>
@@ -29441,7 +29557,7 @@
         <v>43</v>
       </c>
       <c r="M123" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N123" s="2" t="s">
         <v>751</v>
@@ -29487,13 +29603,13 @@
         <v>759</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>1276</v>
+        <v>1294</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>760</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>1277</v>
+        <v>1295</v>
       </c>
       <c r="I125" s="1" t="s">
         <v>762</v>
@@ -29508,7 +29624,7 @@
         <v>43</v>
       </c>
       <c r="M125" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N125" s="2" t="s">
         <v>764</v>
@@ -29607,7 +29723,7 @@
         <v>44885.0</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>1278</v>
+        <v>1296</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>776</v>
@@ -29628,7 +29744,7 @@
         <v>204</v>
       </c>
       <c r="M130" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N130" s="2" t="s">
         <v>780</v>
@@ -29672,13 +29788,13 @@
         <v>16493.0</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>1279</v>
+        <v>1297</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>787</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>1280</v>
+        <v>1298</v>
       </c>
       <c r="I132" s="1" t="s">
         <v>789</v>
@@ -29693,7 +29809,7 @@
         <v>26</v>
       </c>
       <c r="M132" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N132" s="2" t="s">
         <v>791</v>
@@ -29737,7 +29853,7 @@
         <v>798</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>1281</v>
+        <v>1299</v>
       </c>
       <c r="G134" s="2" t="s">
         <v>799</v>
@@ -29838,7 +29954,7 @@
         <v>813</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>1282</v>
+        <v>1300</v>
       </c>
       <c r="G138" s="1" t="s">
         <v>814</v>
@@ -29859,7 +29975,7 @@
         <v>61</v>
       </c>
       <c r="M138" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N138" s="2" t="s">
         <v>818</v>
@@ -29903,7 +30019,7 @@
         <v>825</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>1283</v>
+        <v>1301</v>
       </c>
       <c r="G140" s="1" t="s">
         <v>826</v>
@@ -29912,7 +30028,7 @@
         <v>827</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>1284</v>
+        <v>1302</v>
       </c>
       <c r="J140" s="1" t="s">
         <v>829</v>
@@ -29924,7 +30040,7 @@
         <v>61</v>
       </c>
       <c r="M140" s="1" t="s">
-        <v>1285</v>
+        <v>1303</v>
       </c>
       <c r="N140" s="2" t="s">
         <v>830</v>
@@ -29971,7 +30087,7 @@
         <v>9420.0</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>1286</v>
+        <v>1304</v>
       </c>
       <c r="G142" s="1" t="s">
         <v>839</v>
@@ -29980,7 +30096,7 @@
         <v>840</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>1287</v>
+        <v>1305</v>
       </c>
       <c r="J142" s="1" t="s">
         <v>60</v>
@@ -29992,7 +30108,7 @@
         <v>204</v>
       </c>
       <c r="M142" s="1" t="s">
-        <v>1285</v>
+        <v>1303</v>
       </c>
       <c r="N142" s="2" t="s">
         <v>842</v>
@@ -30037,7 +30153,7 @@
         <v>850</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>1288</v>
+        <v>1306</v>
       </c>
       <c r="G144" s="1" t="s">
         <v>851</v>
@@ -30058,7 +30174,7 @@
         <v>43</v>
       </c>
       <c r="M144" s="1" t="s">
-        <v>1285</v>
+        <v>1303</v>
       </c>
       <c r="N144" s="2" t="s">
         <v>854</v>
@@ -30103,13 +30219,13 @@
         <v>862</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>1289</v>
+        <v>1307</v>
       </c>
       <c r="G146" s="1" t="s">
         <v>863</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>1290</v>
+        <v>1308</v>
       </c>
       <c r="I146" s="2" t="s">
         <v>865</v>
@@ -30124,7 +30240,7 @@
         <v>43</v>
       </c>
       <c r="M146" s="1" t="s">
-        <v>1285</v>
+        <v>1303</v>
       </c>
       <c r="N146" s="2" t="s">
         <v>866</v>
@@ -30167,10 +30283,10 @@
         <v>16019.0</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>1291</v>
+        <v>1309</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>1292</v>
+        <v>1310</v>
       </c>
       <c r="H148" s="1" t="s">
         <v>874</v>
@@ -30188,7 +30304,7 @@
         <v>204</v>
       </c>
       <c r="M148" s="1" t="s">
-        <v>1285</v>
+        <v>1303</v>
       </c>
       <c r="N148" s="2" t="s">
         <v>876</v>
@@ -30233,7 +30349,7 @@
         <v>254931.0</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>1293</v>
+        <v>1311</v>
       </c>
       <c r="G150" s="1" t="s">
         <v>884</v>
@@ -30245,7 +30361,7 @@
         <v>886</v>
       </c>
       <c r="J150" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K150" s="1" t="s">
         <v>25</v>
@@ -30254,7 +30370,7 @@
         <v>204</v>
       </c>
       <c r="M150" s="1" t="s">
-        <v>1285</v>
+        <v>1303</v>
       </c>
       <c r="N150" s="2" t="s">
         <v>887</v>
@@ -30297,16 +30413,16 @@
         <v>25858.0</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>1294</v>
+        <v>1312</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>894</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>1295</v>
+        <v>1313</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>1296</v>
+        <v>1314</v>
       </c>
       <c r="J152" s="1" t="s">
         <v>60</v>
@@ -30318,7 +30434,7 @@
         <v>204</v>
       </c>
       <c r="M152" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N152" s="2" t="s">
         <v>897</v>
@@ -30362,16 +30478,16 @@
         <v>904</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>1297</v>
+        <v>1315</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>1298</v>
+        <v>1316</v>
       </c>
       <c r="H154" s="1" t="s">
         <v>906</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>1299</v>
+        <v>1317</v>
       </c>
       <c r="J154" s="1" t="s">
         <v>908</v>
@@ -30383,7 +30499,7 @@
         <v>204</v>
       </c>
       <c r="M154" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="N154" s="2" t="s">
         <v>909</v>
@@ -30447,7 +30563,7 @@
         <v>43</v>
       </c>
       <c r="M156" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="157">
@@ -30482,7 +30598,7 @@
         <v>38222.0</v>
       </c>
       <c r="F158" s="14" t="s">
-        <v>1300</v>
+        <v>1318</v>
       </c>
       <c r="G158" s="14" t="s">
         <v>925</v>
@@ -30503,7 +30619,7 @@
         <v>204</v>
       </c>
       <c r="M158" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="159">
@@ -30540,10 +30656,10 @@
         <v>933</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>1301</v>
+        <v>1319</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>1302</v>
+        <v>1320</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>935</v>
@@ -30561,7 +30677,7 @@
         <v>204</v>
       </c>
       <c r="M160" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="161">
@@ -30636,7 +30752,7 @@
         <v>1551.0</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>1303</v>
+        <v>1321</v>
       </c>
       <c r="G164" s="1" t="s">
         <v>947</v>
@@ -30657,7 +30773,7 @@
         <v>204</v>
       </c>
       <c r="M164" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="165">
@@ -30692,10 +30808,10 @@
         <v>2352.0</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>1304</v>
+        <v>1322</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>1305</v>
+        <v>1323</v>
       </c>
       <c r="H166" s="1" t="s">
         <v>955</v>
@@ -30713,7 +30829,7 @@
         <v>43</v>
       </c>
       <c r="M166" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="167">
@@ -30750,10 +30866,10 @@
         <v>963</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>1306</v>
+        <v>1324</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>1307</v>
+        <v>1325</v>
       </c>
       <c r="H168" s="1" t="s">
         <v>965</v>
@@ -30771,7 +30887,7 @@
         <v>43</v>
       </c>
       <c r="M168" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="169">
@@ -30806,7 +30922,7 @@
         <v>971</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>1308</v>
+        <v>1326</v>
       </c>
       <c r="G170" s="1" t="s">
         <v>972</v>
@@ -30827,7 +30943,7 @@
         <v>976</v>
       </c>
       <c r="M170" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="171">
@@ -30898,13 +31014,13 @@
         <v>2015.0</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>1309</v>
+        <v>1327</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>1310</v>
+        <v>1328</v>
       </c>
       <c r="H174" s="1" t="s">
-        <v>1311</v>
+        <v>1329</v>
       </c>
       <c r="I174" s="1" t="s">
         <v>986</v>
@@ -30919,7 +31035,7 @@
         <v>43</v>
       </c>
       <c r="M174" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="175">
@@ -30975,7 +31091,7 @@
         <v>4072.0</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>1312</v>
+        <v>1330</v>
       </c>
       <c r="G177" s="1" t="s">
         <v>994</v>
@@ -30984,7 +31100,7 @@
         <v>995</v>
       </c>
       <c r="I177" s="1" t="s">
-        <v>1313</v>
+        <v>1331</v>
       </c>
       <c r="J177" s="1" t="s">
         <v>694</v>
@@ -30996,7 +31112,7 @@
         <v>43</v>
       </c>
       <c r="M177" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="178">
@@ -31031,7 +31147,7 @@
         <v>40921.0</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>1314</v>
+        <v>1332</v>
       </c>
       <c r="G179" s="1"/>
       <c r="H179" s="1" t="s">
@@ -31106,7 +31222,7 @@
         <v>1012</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>1315</v>
+        <v>1333</v>
       </c>
       <c r="G182" s="1" t="s">
         <v>1013</v>
@@ -31115,7 +31231,7 @@
         <v>1014</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>1316</v>
+        <v>1334</v>
       </c>
       <c r="J182" s="1" t="s">
         <v>1016</v>
@@ -31127,7 +31243,7 @@
         <v>204</v>
       </c>
       <c r="M182" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="183">
@@ -31162,10 +31278,10 @@
         <v>1022</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>1317</v>
+        <v>1335</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>1318</v>
+        <v>1336</v>
       </c>
       <c r="H184" s="1" t="s">
         <v>1024</v>
@@ -31183,7 +31299,7 @@
         <v>43</v>
       </c>
       <c r="M184" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="185">
@@ -31256,13 +31372,13 @@
         <v>1035</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>1319</v>
+        <v>1337</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>1320</v>
+        <v>1338</v>
       </c>
       <c r="H188" s="1" t="s">
-        <v>1321</v>
+        <v>1339</v>
       </c>
       <c r="I188" s="1" t="s">
         <v>1038</v>
@@ -31277,7 +31393,7 @@
         <v>204</v>
       </c>
       <c r="M188" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="189">
@@ -31314,16 +31430,16 @@
         <v>1045</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>1322</v>
+        <v>1340</v>
       </c>
       <c r="G190" s="1" t="s">
         <v>1046</v>
       </c>
       <c r="H190" s="1" t="s">
-        <v>1323</v>
+        <v>1341</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>1324</v>
+        <v>1342</v>
       </c>
       <c r="J190" s="1" t="s">
         <v>1049</v>
@@ -31335,7 +31451,7 @@
         <v>43</v>
       </c>
       <c r="M190" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="191">
@@ -31374,13 +31490,13 @@
         <v>1056</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>1325</v>
+        <v>1343</v>
       </c>
       <c r="G192" s="1" t="s">
         <v>1057</v>
       </c>
       <c r="H192" s="1" t="s">
-        <v>1326</v>
+        <v>1344</v>
       </c>
       <c r="I192" s="1" t="s">
         <v>1059</v>
@@ -31395,7 +31511,7 @@
         <v>26</v>
       </c>
       <c r="M192" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="193">
@@ -31430,10 +31546,10 @@
         <v>1065</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>1327</v>
+        <v>1345</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>1328</v>
+        <v>1346</v>
       </c>
       <c r="H194" s="1" t="s">
         <v>1067</v>
@@ -31451,7 +31567,7 @@
         <v>43</v>
       </c>
       <c r="M194" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="195">
@@ -31507,16 +31623,16 @@
         <v>1077</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>1329</v>
+        <v>1347</v>
       </c>
       <c r="G197" s="1" t="s">
-        <v>1330</v>
+        <v>1348</v>
       </c>
       <c r="H197" s="1" t="s">
         <v>1079</v>
       </c>
       <c r="I197" s="1" t="s">
-        <v>1331</v>
+        <v>1349</v>
       </c>
       <c r="J197" s="1" t="s">
         <v>817</v>
@@ -31528,7 +31644,7 @@
         <v>43</v>
       </c>
       <c r="M197" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="198">
@@ -31565,7 +31681,7 @@
         <v>1086</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>1332</v>
+        <v>1350</v>
       </c>
       <c r="G199" s="1" t="s">
         <v>1087</v>
@@ -31586,7 +31702,7 @@
         <v>43</v>
       </c>
       <c r="M199" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="200">
@@ -31640,7 +31756,7 @@
         <v>1097</v>
       </c>
       <c r="F202" s="1" t="s">
-        <v>1333</v>
+        <v>1351</v>
       </c>
       <c r="G202" s="1" t="s">
         <v>1098</v>
@@ -31661,7 +31777,7 @@
         <v>204</v>
       </c>
       <c r="M202" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="203">
@@ -31696,13 +31812,13 @@
         <v>2624.0</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>1334</v>
+        <v>1352</v>
       </c>
       <c r="G204" s="1" t="s">
         <v>1106</v>
       </c>
       <c r="H204" s="1" t="s">
-        <v>1335</v>
+        <v>1353</v>
       </c>
       <c r="I204" s="1" t="s">
         <v>1108</v>
@@ -31717,7 +31833,7 @@
         <v>26</v>
       </c>
       <c r="M204" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="205">
@@ -31752,7 +31868,7 @@
         <v>1114</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>1336</v>
+        <v>1354</v>
       </c>
       <c r="G206" s="1" t="s">
         <v>1115</v>
@@ -31771,7 +31887,7 @@
         <v>26</v>
       </c>
       <c r="M206" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="207">
@@ -31804,7 +31920,7 @@
         <v>1120</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>1337</v>
+        <v>1355</v>
       </c>
       <c r="G208" s="1" t="s">
         <v>1121</v>
@@ -31821,7 +31937,7 @@
         <v>43</v>
       </c>
       <c r="M208" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="209">
@@ -31856,7 +31972,7 @@
         <v>12049.0</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>1338</v>
+        <v>1356</v>
       </c>
       <c r="G210" s="1" t="s">
         <v>1127</v>
@@ -31865,7 +31981,7 @@
         <v>1128</v>
       </c>
       <c r="I210" s="1" t="s">
-        <v>1339</v>
+        <v>1357</v>
       </c>
       <c r="J210" s="1" t="s">
         <v>1130</v>
@@ -31877,7 +31993,7 @@
         <v>43</v>
       </c>
       <c r="M210" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="211">
@@ -31912,19 +32028,19 @@
         <v>1135</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>1340</v>
+        <v>1358</v>
       </c>
       <c r="G212" s="1" t="s">
         <v>1136</v>
       </c>
       <c r="H212" s="1" t="s">
-        <v>1341</v>
+        <v>1359</v>
       </c>
       <c r="I212" s="1" t="s">
         <v>1138</v>
       </c>
       <c r="J212" s="17" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
       <c r="K212" s="1" t="s">
         <v>25</v>
@@ -31933,7 +32049,7 @@
         <v>26</v>
       </c>
       <c r="M212" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="213">
@@ -31987,7 +32103,7 @@
         <v>1145</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>1342</v>
+        <v>1360</v>
       </c>
       <c r="G215" s="1" t="s">
         <v>1146</v>
@@ -32008,7 +32124,7 @@
         <v>43</v>
       </c>
       <c r="M215" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="216">
@@ -32096,7 +32212,7 @@
         <v>1157</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>1343</v>
+        <v>1361</v>
       </c>
       <c r="G220" s="1" t="s">
         <v>1158</v>
@@ -32117,7 +32233,7 @@
         <v>204</v>
       </c>
       <c r="M220" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="221">
@@ -32154,7 +32270,7 @@
         <v>57147.0</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>1344</v>
+        <v>1362</v>
       </c>
       <c r="G222" s="1" t="s">
         <v>1166</v>
@@ -32175,7 +32291,7 @@
         <v>43</v>
       </c>
       <c r="M222" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="223">
@@ -32210,7 +32326,7 @@
         <v>1173</v>
       </c>
       <c r="F224" s="1" t="s">
-        <v>1345</v>
+        <v>1363</v>
       </c>
       <c r="G224" s="1" t="s">
         <v>415</v>
@@ -32229,7 +32345,7 @@
         <v>204</v>
       </c>
       <c r="M224" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="225">
@@ -32255,10 +32371,10 @@
         <v>836</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="E226" s="6"/>
       <c r="F226" s="6"/>
@@ -32266,7 +32382,7 @@
       <c r="H226" s="6"/>
       <c r="I226" s="6"/>
       <c r="J226" s="1" t="s">
-        <v>1179</v>
+        <v>1183</v>
       </c>
       <c r="K226" s="1" t="s">
         <v>44</v>
@@ -32275,7 +32391,7 @@
         <v>204</v>
       </c>
       <c r="M226" s="1" t="s">
-        <v>1195</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="227">
@@ -32295,11 +32411,11 @@
     </row>
     <row r="228">
       <c r="A228" s="1" t="s">
-        <v>1180</v>
+        <v>1184</v>
       </c>
       <c r="B228" s="6"/>
       <c r="C228" s="4" t="s">
-        <v>1181</v>
+        <v>1185</v>
       </c>
       <c r="D228" s="6"/>
       <c r="E228" s="6"/>
@@ -32329,7 +32445,7 @@
     </row>
     <row r="230">
       <c r="A230" s="1" t="s">
-        <v>1182</v>
+        <v>1186</v>
       </c>
       <c r="B230" s="6"/>
       <c r="C230" s="6"/>
@@ -32361,7 +32477,7 @@
     </row>
     <row r="232">
       <c r="A232" s="1" t="s">
-        <v>1183</v>
+        <v>1187</v>
       </c>
       <c r="B232" s="6"/>
       <c r="C232" s="6"/>
@@ -32378,7 +32494,7 @@
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
-        <v>1184</v>
+        <v>1188</v>
       </c>
       <c r="B233" s="6"/>
       <c r="C233" s="6"/>
@@ -32395,7 +32511,7 @@
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
-        <v>1185</v>
+        <v>1189</v>
       </c>
       <c r="B234" s="6"/>
       <c r="C234" s="6"/>
@@ -32427,7 +32543,7 @@
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
-        <v>1186</v>
+        <v>1190</v>
       </c>
       <c r="B236" s="6"/>
       <c r="C236" s="6"/>
@@ -32444,7 +32560,7 @@
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
-        <v>1187</v>
+        <v>1191</v>
       </c>
       <c r="B237" s="6"/>
       <c r="C237" s="6"/>
@@ -32461,7 +32577,7 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>1188</v>
+        <v>1192</v>
       </c>
       <c r="B238" s="6"/>
       <c r="C238" s="6"/>
@@ -32478,7 +32594,7 @@
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
-        <v>1189</v>
+        <v>1193</v>
       </c>
       <c r="B239" s="6"/>
       <c r="C239" s="6"/>
@@ -32495,7 +32611,7 @@
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>1190</v>
+        <v>1199</v>
       </c>
       <c r="B240" s="6"/>
       <c r="C240" s="6"/>

</xml_diff>

<commit_message>
BP-644 speialized classes made and data migrations fix
</commit_message>
<xml_diff>
--- a/assets/extData.xlsx
+++ b/assets/extData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5727" uniqueCount="1878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5732" uniqueCount="1899">
   <si>
     <t>Полное название</t>
   </si>
@@ -91,7 +91,7 @@
     <t>Многопрофильный лицей со специализированными классами при НИУ ВШЭ, МГМУ имения И.М.Сеченова и МГУ имени М.В.Ломносова</t>
   </si>
   <si>
-    <t>был открыт как экспериментальный лицей с востоковедным уклоном при ИСАА МГУ в 1991 году; с 2011 по 2015 крепко удерживает лидерство среди московских школ;реализует программу Дополнительного образования для школьников 13-18 лет, где ведется подготовка к олимпиадам; при лицее работает «Открытая школа»; ежегодно летом две естественнонаучные экспедиции выезжают на Белое море и на озеро Байкал;
+    <t>был открыт как экспериментальный лицей с востоковедческим уклоном при ИСАА МГУ в 1991 году; с 2011 по 2015 крепко удерживает лидерство среди московских школ;реализует программу Дополнительного образования для школьников 13-18 лет, где ведется подготовка к олимпиадам; при лицее работает «Открытая школа»; ежегодно летом две естественнонаучные экспедиции выезжают на Белое море и на озеро Байкал;
 </t>
   </si>
   <si>
@@ -600,7 +600,7 @@
     <t xml:space="preserve">Школа полного дня со спортивным уклоном и сильным физико-математическим направлением </t>
   </si>
   <si>
-    <t>При школе действует содружество математиков- творческая лаборатория "2х2"; на Первой международной олимпиаде по экспериментальной физике для старшеклассников сразу 10 учеников школы заняли призовые места; при школе работают курсы интенсивной подготовки для школьников «Умный и ещё умнее».
+    <t>При школе действует содружество математиков - творческая лаборатория "2х2"; на Первой международной олимпиаде по экспериментальной физике для старшеклассников сразу 10 учеников школы заняли призовые места; при школе работают курсы интенсивной подготовки для школьников «Умный и ещё умнее».
 </t>
   </si>
   <si>
@@ -959,7 +959,7 @@
     <t>Многопрофильный лицей с курсами по компьютерным технологиям, телевизионному мастерству и основам режиссуры</t>
   </si>
   <si>
-    <t>Лицей сотрудничает с Гуманитарным институтом телевидения и радиовещания, НИТУ МИСиС, НИУ ВШЭ, МГУ, МГПУ; лицей является площадкой по проведению Олимпиады школьников "Нанотехнологии - прорыв в будущее; победитель второго этапа проекта "Школа Новых технологий"
+    <t>Лицей сотрудничает с Гуманитарным институтом телевидения и радиовещания, НИТУ МИСиС, НИУ ВШЭ, МГУ, МГПУ; лицей является площадкой по проведению Олимпиады школьников "Нанотехнологии - прорыв в будущее"; победитель второго этапа проекта "Школа Новых технологий"
 </t>
   </si>
   <si>
@@ -1056,7 +1056,7 @@
     <t>Школа с сильным физико-математическим подразделением, созданная учеными Курчатовского института</t>
   </si>
   <si>
-    <t xml:space="preserve">Основана в 1991 году при поддержке Центра компьютерного обучения Курчатовского института; ежегодно совместно с НИЦ "Курчатовский институт" и ФНБИК МФТИ проводит Олимпиаду "Курчатов" по математике и физике; занятия в школе ведут научные сотрудники НИЦ «Курчатовский Институт»; В программу преподавания физики и математики включено выполнение заданий Заочной физико-технической школы (ЗФТШ) МФТИ. По завершении обучения выпускники физико-математических классов наряду с аттестатом о среднем образовании получают и диплом об окончании ЗФТШ стандартного образца.
+    <t xml:space="preserve">Ежегодно совместно с НИЦ "Курчатовский институт"  проводит Олимпиаду "Курчатов" по математике и физике; занятия в школе ведут научные сотрудники НИЦ «Курчатовский Институт»; В программу обучения включено выполнение заданий Заочной физико-технической школы МФТИ; Выпускники физико-математических классов получают диплом об окончании заочной физико-технической школы МФТИ
  </t>
   </si>
   <si>
@@ -4196,7 +4196,7 @@
     <t>http://lyc1564.mskobr.ru/</t>
   </si>
   <si>
-    <t>http://vk.com/club1855835 - (-: лицей 1564 :-)
+    <t>http://vk.com/club1855835 - (: лицей 1564 :)
 </t>
   </si>
   <si>
@@ -5825,7 +5825,7 @@
 10</t>
   </si>
   <si>
-    <t xml:space="preserve">Школа Андрея Миронова и Эдварда Радзинского, с распределенным лицеем и углубленным изучением предметов </t>
+    <t>Школа Андрея Миронова и Эдварда Радзинского, с распределенным лицеем и углубленным изучением английского языка, музыки и хореографии</t>
   </si>
   <si>
     <t>при школе действуют классы с литературно-театральным уклоном; сотрудничает с ВТУ имени М.С.Щепкина, с РУДН; организованы химико-технологические классы при Академии тонкой химической технологии имени М.В.Ломоносова; школа № 1219 является базой Московского архитектурного института</t>
@@ -6358,7 +6358,7 @@
     <t>Школа с программой международного бакалавриата и углубленным изучением испанского языка</t>
   </si>
   <si>
-    <t>сотрудничает с Институтом Сервантеса в Москве; победитель Приоритетного национального проекта «Образование";</t>
+    <t>сотрудничает с Институтом Сервантеса в Москве; победитель Приоритетного национального проекта "Образование";</t>
   </si>
   <si>
     <t>1600 руб./мес. - за три часа; 3200 руб./мес. - за шесть часов</t>
@@ -6512,7 +6512,7 @@
     <t xml:space="preserve">Школа-лауреат Гранта Мэра Москвы с программой международного бакалавриата и своим гольф-клубом </t>
   </si>
   <si>
-    <t xml:space="preserve">в 2013 году признан лучшей базовой образовательной организацией МГТУ им. Н.Э. Баумана; сотрудничает с МГТУ имени Н.Э.Баумана; МАДИ, МГПУ; школа реализует программу международного бакалавриата; при школе работает клуб "Юных журналистов", который выпускает свою газеты и журнал;участница Федеральной инновационной площадки «Школьная лига» </t>
+    <t xml:space="preserve">в 2013 году признан лучшей базовой образовательной организацией МГТУ им. Н.Э. Баумана; сотрудничает с МГТУ имени Н.Э.Баумана, МАДИ, МГПУ; школа реализует программу международного бакалавриата; при школе работает клуб "Юных журналистов", который выпускает свою газеты и журнал;участница Федеральной инновационной площадки «Школьная лига» </t>
   </si>
   <si>
     <t>2199 руб./мес.</t>
@@ -6660,7 +6660,7 @@
     <t>Школа со своим телевидением, программой лингвистических стажировок в Великобритании и на Мальте</t>
   </si>
   <si>
-    <t>есть своей школьное телевидение; в школе реализуется программа стажировок в Великобритании и на Мальте; победитель второго этапа проекта "Школа Новых Технологий"</t>
+    <t>есть свое школьное телевидение; в школе реализуется программа стажировок в Великобритании и на Мальте; победитель второго этапа проекта "Школа Новых Технологий"</t>
   </si>
   <si>
     <t>Северный административный округ;
@@ -7340,7 +7340,7 @@
     <t>Лицей с занятиями по флэш-анимации, системному программированию и робототехнике</t>
   </si>
   <si>
-    <t xml:space="preserve">ассоциированная школа ЮНЕСКО; Сотрудничает с Microsoft, ABBY, 1C и Лабораторией Касперского; сотрудничает с факультетом ВМК МГУ, РГУ нефти и газа имени И.М.Губкина; </t>
+    <t xml:space="preserve">ассоциированная школа ЮНЕСКО; Сотрудничает с Microsoft, ABBYY, 1C и Лабораторией Касперского; сотрудничает с факультетом ВМК МГУ, РГУ нефти и газа имени И.М.Губкина; </t>
   </si>
   <si>
     <t>Юго-Западный административный округ;
@@ -7845,7 +7845,7 @@
 10</t>
   </si>
   <si>
-    <t>Школа с профильными классами при МГТУ имени Н.Э.Баумана, физическом факульетете МГУ, МГУПИ и занятиями по роботехнике</t>
+    <t>Школа с профильными классами при МГТУ имени Н.Э.Баумана, физическом факультете МГУ, МГУПИ и занятиями по роботехнике</t>
   </si>
   <si>
     <t>Лауреат Гранта Мэра Москвы в сфере образования;  есть своя газета "Вектор 444"</t>
@@ -8011,18 +8011,11 @@
 1337 (цо 1099)</t>
   </si>
   <si>
-    <t>технлогический; социально-экономический; социально-гуманитарный; универсальный
+    <t>технологический; социально-экономический; социально-гуманитарный; универсальный
 10</t>
   </si>
   <si>
     <t>Лицей с углубленным изучением информатики, математики, физики и курсами по робототехнике</t>
-  </si>
-  <si>
-    <t>участник проекта "Школа Новых Технологий"; лауреат Гранта Мэра Москвы в сфере образования; базовое профильное учреждение МГТУ им. Н.Э.Баумана и НИУ ВШЭ; лауреат Всероссийского конкурса "Лучшие школы России"; сотрудничает с МГУ, МФТИ, МГТУ имени Н.Э.Баумана, НИЯУ МИФИ, АКадиемией ФСБ РФ; в Лицее организована группа робототехнического творчества "Роболит".
-</t>
-  </si>
-  <si>
-    <t>бесплатно?</t>
   </si>
   <si>
     <t>Северо-Восточный административный округ;
@@ -8201,10 +8194,26 @@
 10</t>
   </si>
   <si>
-    <t>Женский кадетский корпус со школами журналистики, политологии и этикета и стипениями воспитанницам</t>
+    <t>Женский кадетский корпус со школами журналистики, политологии и этикета и стипендиями воспитанницам</t>
   </si>
   <si>
     <t>сотрудничает с МГТУ имение Баумана; ежегодно  проводится научно-практическая конференция «Взгляд в будущее»; при пансионе действует Летняя школа</t>
+  </si>
+  <si>
+    <t>Северо-Западный административный округ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">район Хорошейвский </t>
+  </si>
+  <si>
+    <t>ул. Поликарпова, 21
+</t>
+  </si>
+  <si>
+    <t>7(495) 946-02-95</t>
+  </si>
+  <si>
+    <t>Максимова Лариса Юрьевна</t>
   </si>
   <si>
     <t>Государственное бюджетное общеобразовательное учреждение города Москвы "Лицей № 1553 имени В.И. Вернадского"</t>
@@ -8274,8 +8283,7 @@
     <t xml:space="preserve">Многопрофильная школа в Беляево с кадетскими классами и курсами Web-дизайна </t>
   </si>
   <si>
-    <t xml:space="preserve">сотрудничает со Спецшколой им. Чан Фу  (Вьетнам) и со школой Берты-фон-Зюттнер (Германия)
-в школе действует секция тхэквондо </t>
+    <t xml:space="preserve">сотрудничает со Спецшколой им. Чан Фу  (Вьетнам) и со школой Берты-фон-Зюттнер (Германия);в школе действует секция тхэквондо </t>
   </si>
   <si>
     <t>Юго-Западный административный округ;
@@ -8570,6 +8578,26 @@
 </t>
   </si>
   <si>
+    <t>был открыт как экспериментальный лицей с востоковедным уклоном при ИСАА МГУ в 1991 году; с 2011 по 2015 крепко удерживает лидерство среди московских школ;реализует программу Дополнительного образования для школьников 13-18 лет, где ведется подготовка к олимпиадам; при лицее работает «Открытая школа»; ежегодно летом две естественнонаучные экспедиции выезжают на Белое море и на озеро Байкал;
+</t>
+  </si>
+  <si>
+    <t>При школе действует содружество математиков- творческая лаборатория "2х2"; на Первой международной олимпиаде по экспериментальной физике для старшеклассников сразу 10 учеников школы заняли призовые места; при школе работают курсы интенсивной подготовки для школьников «Умный и ещё умнее».
+</t>
+  </si>
+  <si>
+    <t>Лицей сотрудничает с Гуманитарным институтом телевидения и радиовещания, НИТУ МИСиС, НИУ ВШЭ, МГУ, МГПУ; лицей является площадкой по проведению Олимпиады школьников "Нанотехнологии - прорыв в будущее; победитель второго этапа проекта "Школа Новых технологий"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Основана в 1991 году при поддержке Центра компьютерного обучения Курчатовского института; ежегодно совместно с НИЦ "Курчатовский институт" и ФНБИК МФТИ проводит Олимпиаду "Курчатов" по математике и физике; занятия в школе ведут научные сотрудники НИЦ «Курчатовский Институт»; В программу преподавания физики и математики включено выполнение заданий Заочной физико-технической школы (ЗФТШ) МФТИ. По завершении обучения выпускники физико-математических классов наряду с аттестатом о среднем образовании получают и диплом об окончании ЗФТШ стандартного образца.
+ </t>
+  </si>
+  <si>
+    <t>https://vk.com/sch192- Школа №192
+</t>
+  </si>
+  <si>
     <t>Юго-Западный административный округ;
 Юго-Западный административный округ;
 Юго-Западный административный округ;
@@ -8610,6 +8638,62 @@
 Начальное, основное и среднее образование</t>
   </si>
   <si>
+    <t>http://vk.com/club1855835 - (-: лицей 1564 :-)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Школа Андрея Миронова и Эдварда Радзинского, с распределенным лицеем и углубленным изучением предметов </t>
+  </si>
+  <si>
+    <t>сотрудничает с Институтом Сервантеса в Москве; победитель Приоритетного национального проекта «Образование";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">в 2013 году признан лучшей базовой образовательной организацией МГТУ им. Н.Э. Баумана; сотрудничает с МГТУ имени Н.Э.Баумана; МАДИ, МГПУ; школа реализует программу международного бакалавриата; при школе работает клуб "Юных журналистов", который выпускает свою газеты и журнал;участница Федеральной инновационной площадки «Школьная лига» </t>
+  </si>
+  <si>
+    <t>есть своей школьное телевидение; в школе реализуется программа стажировок в Великобритании и на Мальте; победитель второго этапа проекта "Школа Новых Технологий"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ассоциированная школа ЮНЕСКО; Сотрудничает с Microsoft, ABBY, 1C и Лабораторией Касперского; сотрудничает с факультетом ВМК МГУ, РГУ нефти и газа имени И.М.Губкина; </t>
+  </si>
+  <si>
+    <t>Школа с профильными классами при МГТУ имени Н.Э.Баумана, физическом факульетете МГУ, МГУПИ и занятиями по роботехнике</t>
+  </si>
+  <si>
+    <t>технлогический; социально-экономический; социально-гуманитарный; универсальный
+10</t>
+  </si>
+  <si>
+    <t>участник проекта "Школа Новых Технологий"; лауреат Гранта Мэра Москвы в сфере образования; базовое профильное учреждение МГТУ им. Н.Э.Баумана и НИУ ВШЭ; лауреат Всероссийского конкурса "Лучшие школы России"; сотрудничает с МГУ, МФТИ, МГТУ имени Н.Э.Баумана, НИЯУ МИФИ, АКадиемией ФСБ РФ; в Лицее организована группа робототехнического творчества "Роболит".
+</t>
+  </si>
+  <si>
+    <t>бесплатно?</t>
+  </si>
+  <si>
+    <t>Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ;
+Северо-Западный административный округ
+</t>
+  </si>
+  <si>
+    <t>Женский кадетский корпус со школами журналистики, политологии и этикета и стипениями воспитанницам</t>
+  </si>
+  <si>
     <t>Юго-Восточный административный округ;
 Юго-Восточный административный округ;
 Юго-Восточный административный округ;
@@ -8644,6 +8728,10 @@
   </si>
   <si>
     <t>http://mpgv.mskobr.ru/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">сотрудничает со Спецшколой им. Чан Фу  (Вьетнам) и со школой Берты-фон-Зюттнер (Германия)
+в школе действует секция тхэквондо </t>
   </si>
   <si>
     <t>2376 руб./мес. (18 р/час)</t>
@@ -10235,7 +10323,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
@@ -10296,6 +10384,9 @@
     </xf>
     <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
@@ -12657,7 +12748,7 @@
       <c r="C75" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="D75" s="7"/>
+      <c r="D75" s="21"/>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
       <c r="G75" s="7"/>
@@ -12904,7 +12995,7 @@
       <c r="B83" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="C83" s="21" t="s">
+      <c r="C83" s="22" t="s">
         <v>477</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -13184,7 +13275,7 @@
       <c r="L90" s="7"/>
     </row>
     <row r="91">
-      <c r="A91" s="22" t="s">
+      <c r="A91" s="23" t="s">
         <v>538</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -13240,7 +13331,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="22"/>
+      <c r="A92" s="23"/>
       <c r="B92" s="1"/>
       <c r="C92" s="4" t="s">
         <v>553</v>
@@ -13258,7 +13349,7 @@
       <c r="L92" s="7"/>
     </row>
     <row r="93">
-      <c r="A93" s="22"/>
+      <c r="A93" s="23"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="15" t="s">
@@ -14032,7 +14123,7 @@
       <c r="N114" s="2" t="s">
         <v>709</v>
       </c>
-      <c r="O114" s="23" t="s">
+      <c r="O114" s="24" t="s">
         <v>710</v>
       </c>
       <c r="P114" s="2" t="s">
@@ -14119,7 +14210,7 @@
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
-      <c r="D117" s="24" t="s">
+      <c r="D117" s="25" t="s">
         <v>729</v>
       </c>
       <c r="E117" s="7"/>
@@ -17880,11 +17971,9 @@
       <c r="G233" s="1" t="s">
         <v>1463</v>
       </c>
-      <c r="H233" s="1" t="s">
-        <v>1464</v>
-      </c>
-      <c r="I233" s="18" t="s">
-        <v>1465</v>
+      <c r="H233" s="1"/>
+      <c r="I233" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="J233" s="1" t="s">
         <v>25</v>
@@ -17896,32 +17985,32 @@
         <v>25</v>
       </c>
       <c r="M233" s="2" t="s">
+        <v>1464</v>
+      </c>
+      <c r="N233" s="2" t="s">
+        <v>1465</v>
+      </c>
+      <c r="O233" s="2" t="s">
         <v>1466</v>
       </c>
-      <c r="N233" s="2" t="s">
+      <c r="P233" s="2" t="s">
         <v>1467</v>
       </c>
-      <c r="O233" s="2" t="s">
+      <c r="Q233" s="2" t="s">
         <v>1468</v>
       </c>
-      <c r="P233" s="2" t="s">
+      <c r="R233" s="2" t="s">
         <v>1469</v>
-      </c>
-      <c r="Q233" s="2" t="s">
-        <v>1470</v>
-      </c>
-      <c r="R233" s="2" t="s">
-        <v>1471</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1"/>
       <c r="B234" s="7"/>
       <c r="C234" s="4" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="E234" s="7"/>
       <c r="F234" s="7"/>
@@ -17934,28 +18023,28 @@
     </row>
     <row r="235">
       <c r="A235" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B235" s="15" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C235" s="4" t="s">
         <v>1474</v>
       </c>
-      <c r="B235" s="15" t="s">
+      <c r="D235" s="1" t="s">
         <v>1475</v>
-      </c>
-      <c r="C235" s="4" t="s">
-        <v>1476</v>
-      </c>
-      <c r="D235" s="1" t="s">
-        <v>1477</v>
       </c>
       <c r="E235" s="1">
         <v>31202.0</v>
       </c>
       <c r="F235" s="1" t="s">
+        <v>1476</v>
+      </c>
+      <c r="G235" s="1" t="s">
+        <v>1477</v>
+      </c>
+      <c r="H235" s="1" t="s">
         <v>1478</v>
-      </c>
-      <c r="G235" s="1" t="s">
-        <v>1479</v>
-      </c>
-      <c r="H235" s="1" t="s">
-        <v>1480</v>
       </c>
       <c r="I235" s="1" t="s">
         <v>60</v>
@@ -17970,48 +18059,48 @@
         <v>25</v>
       </c>
       <c r="M235" s="2" t="s">
+        <v>1479</v>
+      </c>
+      <c r="N235" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="O235" s="2" t="s">
         <v>1481</v>
       </c>
-      <c r="N235" s="2" t="s">
+      <c r="P235" s="2" t="s">
         <v>1482</v>
       </c>
-      <c r="O235" s="2" t="s">
+      <c r="Q235" s="2" t="s">
         <v>1483</v>
       </c>
-      <c r="P235" s="2" t="s">
+      <c r="R235" s="2" t="s">
         <v>1484</v>
-      </c>
-      <c r="Q235" s="2" t="s">
-        <v>1485</v>
-      </c>
-      <c r="R235" s="2" t="s">
-        <v>1486</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C236" s="4" t="s">
         <v>1487</v>
       </c>
-      <c r="B236" s="1" t="s">
+      <c r="D236" s="1" t="s">
         <v>1488</v>
-      </c>
-      <c r="C236" s="4" t="s">
-        <v>1489</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>1490</v>
       </c>
       <c r="E236" s="1">
         <v>1668259.0</v>
       </c>
       <c r="F236" s="1" t="s">
+        <v>1489</v>
+      </c>
+      <c r="G236" s="1" t="s">
+        <v>1490</v>
+      </c>
+      <c r="H236" s="1" t="s">
         <v>1491</v>
-      </c>
-      <c r="G236" s="1" t="s">
-        <v>1492</v>
-      </c>
-      <c r="H236" s="1" t="s">
-        <v>1493</v>
       </c>
       <c r="I236" s="2" t="s">
         <v>1126</v>
@@ -18025,12 +18114,24 @@
       <c r="L236" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="M236" s="2"/>
-      <c r="N236" s="2"/>
-      <c r="O236" s="2"/>
-      <c r="P236" s="2"/>
-      <c r="Q236" s="2"/>
-      <c r="R236" s="2"/>
+      <c r="M236" s="15" t="s">
+        <v>1492</v>
+      </c>
+      <c r="N236" s="2" t="s">
+        <v>1493</v>
+      </c>
+      <c r="O236" s="2" t="s">
+        <v>1494</v>
+      </c>
+      <c r="P236" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q236" s="2" t="s">
+        <v>1495</v>
+      </c>
+      <c r="R236" s="2" t="s">
+        <v>1496</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="7"/>
@@ -18048,28 +18149,28 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>1494</v>
+        <v>1497</v>
       </c>
       <c r="B238" s="15" t="s">
-        <v>1495</v>
+        <v>1498</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>1496</v>
+        <v>1499</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>1497</v>
+        <v>1500</v>
       </c>
       <c r="E238" s="1">
         <v>2700.0</v>
       </c>
       <c r="F238" s="1" t="s">
-        <v>1498</v>
+        <v>1501</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>1499</v>
+        <v>1502</v>
       </c>
       <c r="H238" s="1" t="s">
-        <v>1500</v>
+        <v>1503</v>
       </c>
       <c r="I238" s="1" t="s">
         <v>25</v>
@@ -18084,29 +18185,29 @@
         <v>25</v>
       </c>
       <c r="M238" s="2" t="s">
-        <v>1501</v>
+        <v>1504</v>
       </c>
       <c r="N238" s="2" t="s">
-        <v>1502</v>
+        <v>1505</v>
       </c>
       <c r="O238" s="2" t="s">
-        <v>1503</v>
+        <v>1506</v>
       </c>
       <c r="P238" s="2" t="s">
         <v>127</v>
       </c>
       <c r="Q238" s="2" t="s">
-        <v>1504</v>
+        <v>1507</v>
       </c>
       <c r="R238" s="2" t="s">
-        <v>1505</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1"/>
       <c r="B239" s="15"/>
       <c r="C239" s="4" t="s">
-        <v>1506</v>
+        <v>1509</v>
       </c>
       <c r="D239" s="7"/>
       <c r="E239" s="7"/>
@@ -18120,28 +18221,28 @@
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>1507</v>
+        <v>1510</v>
       </c>
       <c r="B240" s="15" t="s">
-        <v>1508</v>
+        <v>1511</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>1509</v>
+        <v>1512</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>1510</v>
+        <v>1513</v>
       </c>
       <c r="E240" s="1">
         <v>1855.0</v>
       </c>
       <c r="F240" s="1" t="s">
-        <v>1511</v>
+        <v>1514</v>
       </c>
       <c r="G240" s="1" t="s">
-        <v>1512</v>
+        <v>1515</v>
       </c>
       <c r="H240" s="1" t="s">
-        <v>1513</v>
+        <v>1516</v>
       </c>
       <c r="I240" s="1" t="s">
         <v>60</v>
@@ -18156,48 +18257,48 @@
         <v>25</v>
       </c>
       <c r="M240" s="2" t="s">
-        <v>1514</v>
+        <v>1517</v>
       </c>
       <c r="N240" s="2" t="s">
-        <v>1515</v>
+        <v>1518</v>
       </c>
       <c r="O240" s="2" t="s">
-        <v>1516</v>
+        <v>1519</v>
       </c>
       <c r="P240" s="2" t="s">
-        <v>1517</v>
+        <v>1520</v>
       </c>
       <c r="Q240" s="2" t="s">
-        <v>1518</v>
+        <v>1521</v>
       </c>
       <c r="R240" s="2" t="s">
-        <v>1519</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="s">
-        <v>1520</v>
+        <v>1523</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>1521</v>
+        <v>1524</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>1522</v>
+        <v>1525</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>1523</v>
+        <v>1526</v>
       </c>
       <c r="E241" s="1">
         <v>43831.0</v>
       </c>
       <c r="F241" s="1" t="s">
-        <v>1524</v>
+        <v>1527</v>
       </c>
       <c r="G241" s="1" t="s">
-        <v>1525</v>
+        <v>1528</v>
       </c>
       <c r="H241" s="1" t="s">
-        <v>1526</v>
+        <v>1529</v>
       </c>
       <c r="I241" s="1" t="s">
         <v>707</v>
@@ -18212,51 +18313,51 @@
         <v>25</v>
       </c>
       <c r="M241" s="2" t="s">
-        <v>1527</v>
+        <v>1530</v>
       </c>
       <c r="N241" s="2" t="s">
-        <v>1528</v>
+        <v>1531</v>
       </c>
       <c r="O241" s="2" t="s">
-        <v>1529</v>
+        <v>1532</v>
       </c>
       <c r="P241" s="2" t="s">
-        <v>1530</v>
+        <v>1533</v>
       </c>
       <c r="Q241" s="2" t="s">
-        <v>1531</v>
+        <v>1534</v>
       </c>
       <c r="R241" s="2" t="s">
-        <v>1532</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="s">
-        <v>1533</v>
+        <v>1536</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>1534</v>
+        <v>1537</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>1535</v>
+        <v>1538</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>1536</v>
+        <v>1539</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>1537</v>
+        <v>1540</v>
       </c>
       <c r="F242" s="1" t="s">
-        <v>1538</v>
+        <v>1541</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>1539</v>
+        <v>1542</v>
       </c>
       <c r="H242" s="1" t="s">
-        <v>1540</v>
+        <v>1543</v>
       </c>
       <c r="I242" s="1" t="s">
-        <v>1541</v>
+        <v>1544</v>
       </c>
       <c r="J242" s="1" t="s">
         <v>25</v>
@@ -18271,19 +18372,19 @@
         <v>1450</v>
       </c>
       <c r="N242" s="2" t="s">
-        <v>1542</v>
+        <v>1545</v>
       </c>
       <c r="O242" s="2" t="s">
-        <v>1543</v>
+        <v>1546</v>
       </c>
       <c r="P242" s="2" t="s">
-        <v>1544</v>
+        <v>1547</v>
       </c>
       <c r="Q242" s="2" t="s">
-        <v>1545</v>
+        <v>1548</v>
       </c>
       <c r="R242" s="2" t="s">
-        <v>1546</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="243">
@@ -18291,7 +18392,7 @@
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
       <c r="D243" s="1" t="s">
-        <v>1547</v>
+        <v>1550</v>
       </c>
       <c r="E243" s="1"/>
       <c r="F243" s="1"/>
@@ -18304,31 +18405,31 @@
     </row>
     <row r="244">
       <c r="A244" s="1" t="s">
-        <v>1548</v>
+        <v>1551</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>1549</v>
+        <v>1552</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>1550</v>
+        <v>1553</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>1551</v>
+        <v>1554</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>1552</v>
+        <v>1555</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>1553</v>
+        <v>1556</v>
       </c>
       <c r="G244" s="1" t="s">
-        <v>1554</v>
+        <v>1557</v>
       </c>
       <c r="H244" s="1" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
       <c r="I244" s="1" t="s">
-        <v>1556</v>
+        <v>1559</v>
       </c>
       <c r="J244" s="1" t="s">
         <v>25</v>
@@ -18340,22 +18441,22 @@
         <v>25</v>
       </c>
       <c r="M244" s="2" t="s">
-        <v>1557</v>
+        <v>1560</v>
       </c>
       <c r="N244" s="2" t="s">
-        <v>1558</v>
+        <v>1561</v>
       </c>
       <c r="O244" s="2" t="s">
-        <v>1559</v>
+        <v>1562</v>
       </c>
       <c r="P244" s="2" t="s">
-        <v>1560</v>
+        <v>1563</v>
       </c>
       <c r="Q244" s="2" t="s">
-        <v>1561</v>
+        <v>1564</v>
       </c>
       <c r="R244" s="2" t="s">
-        <v>1562</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="245">
@@ -18363,7 +18464,7 @@
       <c r="B245" s="8"/>
       <c r="C245" s="8"/>
       <c r="D245" s="8" t="s">
-        <v>1563</v>
+        <v>1566</v>
       </c>
       <c r="E245" s="8"/>
       <c r="F245" s="8"/>
@@ -30430,7 +30531,7 @@
         <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>1567</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>25</v>
@@ -31143,7 +31244,7 @@
         <v>152</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>153</v>
+        <v>1568</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>154</v>
@@ -31595,7 +31696,7 @@
         <v>238</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>239</v>
+        <v>1569</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>240</v>
@@ -31685,7 +31786,7 @@
         <v>255</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>256</v>
+        <v>1570</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>60</v>
@@ -32624,7 +32725,7 @@
         <v>427</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>428</v>
+        <v>1571</v>
       </c>
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
@@ -32888,7 +32989,7 @@
       <c r="B83" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="C83" s="21" t="s">
+      <c r="C83" s="22" t="s">
         <v>477</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -33133,16 +33234,16 @@
         <v>25</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>1564</v>
+        <v>1572</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>1565</v>
+        <v>1573</v>
       </c>
       <c r="O89" s="2" t="s">
-        <v>1566</v>
+        <v>1574</v>
       </c>
       <c r="P89" s="2" t="s">
-        <v>1567</v>
+        <v>1575</v>
       </c>
       <c r="Q89" s="2" t="s">
         <v>534</v>
@@ -33168,7 +33269,7 @@
       <c r="L90" s="7"/>
     </row>
     <row r="91">
-      <c r="A91" s="22" t="s">
+      <c r="A91" s="23" t="s">
         <v>538</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -33224,7 +33325,7 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="22"/>
+      <c r="A92" s="23"/>
       <c r="B92" s="1"/>
       <c r="C92" s="4" t="s">
         <v>553</v>
@@ -33242,7 +33343,7 @@
       <c r="L92" s="7"/>
     </row>
     <row r="93">
-      <c r="A93" s="22"/>
+      <c r="A93" s="23"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="15" t="s">
@@ -34016,7 +34117,7 @@
       <c r="N114" s="2" t="s">
         <v>709</v>
       </c>
-      <c r="O114" s="23" t="s">
+      <c r="O114" s="24" t="s">
         <v>710</v>
       </c>
       <c r="P114" s="2" t="s">
@@ -34103,7 +34204,7 @@
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
-      <c r="D117" s="24" t="s">
+      <c r="D117" s="25" t="s">
         <v>729</v>
       </c>
       <c r="E117" s="7"/>
@@ -34604,7 +34705,7 @@
         <v>822</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>823</v>
+        <v>1576</v>
       </c>
       <c r="E133" s="1">
         <v>16493.0</v>
@@ -35885,7 +35986,7 @@
         <v>1077</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>1078</v>
+        <v>1577</v>
       </c>
       <c r="H171" s="1" t="s">
         <v>1079</v>
@@ -36417,7 +36518,7 @@
         <v>1177</v>
       </c>
       <c r="H189" s="1" t="s">
-        <v>1178</v>
+        <v>1578</v>
       </c>
       <c r="I189" s="1" t="s">
         <v>1179</v>
@@ -36563,7 +36664,7 @@
         <v>1210</v>
       </c>
       <c r="H193" s="1" t="s">
-        <v>1211</v>
+        <v>1579</v>
       </c>
       <c r="I193" s="1" t="s">
         <v>1212</v>
@@ -36723,7 +36824,7 @@
         <v>1243</v>
       </c>
       <c r="H198" s="1" t="s">
-        <v>1244</v>
+        <v>1580</v>
       </c>
       <c r="I198" s="1" t="s">
         <v>482</v>
@@ -37231,7 +37332,7 @@
         <v>1345</v>
       </c>
       <c r="H213" s="1" t="s">
-        <v>1346</v>
+        <v>1581</v>
       </c>
       <c r="I213" s="1" t="s">
         <v>25</v>
@@ -37720,7 +37821,7 @@
         <v>1432</v>
       </c>
       <c r="G229" s="2" t="s">
-        <v>1433</v>
+        <v>1582</v>
       </c>
       <c r="H229" s="2" t="s">
         <v>1434</v>
@@ -37859,16 +37960,16 @@
         <v>1461</v>
       </c>
       <c r="F233" s="1" t="s">
-        <v>1462</v>
+        <v>1583</v>
       </c>
       <c r="G233" s="1" t="s">
         <v>1463</v>
       </c>
       <c r="H233" s="1" t="s">
-        <v>1464</v>
+        <v>1584</v>
       </c>
       <c r="I233" s="18" t="s">
-        <v>1465</v>
+        <v>1585</v>
       </c>
       <c r="J233" s="1" t="s">
         <v>25</v>
@@ -37880,32 +37981,32 @@
         <v>25</v>
       </c>
       <c r="M233" s="2" t="s">
+        <v>1464</v>
+      </c>
+      <c r="N233" s="2" t="s">
+        <v>1465</v>
+      </c>
+      <c r="O233" s="2" t="s">
         <v>1466</v>
       </c>
-      <c r="N233" s="2" t="s">
+      <c r="P233" s="2" t="s">
         <v>1467</v>
       </c>
-      <c r="O233" s="2" t="s">
+      <c r="Q233" s="2" t="s">
         <v>1468</v>
       </c>
-      <c r="P233" s="2" t="s">
+      <c r="R233" s="2" t="s">
         <v>1469</v>
-      </c>
-      <c r="Q233" s="2" t="s">
-        <v>1470</v>
-      </c>
-      <c r="R233" s="2" t="s">
-        <v>1471</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1"/>
       <c r="B234" s="7"/>
       <c r="C234" s="4" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="E234" s="7"/>
       <c r="F234" s="7"/>
@@ -37918,28 +38019,28 @@
     </row>
     <row r="235">
       <c r="A235" s="1" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B235" s="15" t="s">
+        <v>1473</v>
+      </c>
+      <c r="C235" s="4" t="s">
         <v>1474</v>
       </c>
-      <c r="B235" s="15" t="s">
+      <c r="D235" s="1" t="s">
         <v>1475</v>
-      </c>
-      <c r="C235" s="4" t="s">
-        <v>1476</v>
-      </c>
-      <c r="D235" s="1" t="s">
-        <v>1477</v>
       </c>
       <c r="E235" s="1">
         <v>31202.0</v>
       </c>
       <c r="F235" s="1" t="s">
+        <v>1476</v>
+      </c>
+      <c r="G235" s="1" t="s">
+        <v>1477</v>
+      </c>
+      <c r="H235" s="1" t="s">
         <v>1478</v>
-      </c>
-      <c r="G235" s="1" t="s">
-        <v>1479</v>
-      </c>
-      <c r="H235" s="1" t="s">
-        <v>1480</v>
       </c>
       <c r="I235" s="1" t="s">
         <v>60</v>
@@ -37954,48 +38055,48 @@
         <v>25</v>
       </c>
       <c r="M235" s="2" t="s">
+        <v>1586</v>
+      </c>
+      <c r="N235" s="2" t="s">
+        <v>1480</v>
+      </c>
+      <c r="O235" s="2" t="s">
         <v>1481</v>
       </c>
-      <c r="N235" s="2" t="s">
+      <c r="P235" s="2" t="s">
         <v>1482</v>
       </c>
-      <c r="O235" s="2" t="s">
+      <c r="Q235" s="2" t="s">
         <v>1483</v>
       </c>
-      <c r="P235" s="2" t="s">
+      <c r="R235" s="2" t="s">
         <v>1484</v>
-      </c>
-      <c r="Q235" s="2" t="s">
-        <v>1485</v>
-      </c>
-      <c r="R235" s="2" t="s">
-        <v>1486</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
+        <v>1485</v>
+      </c>
+      <c r="B236" s="1" t="s">
+        <v>1486</v>
+      </c>
+      <c r="C236" s="4" t="s">
         <v>1487</v>
       </c>
-      <c r="B236" s="1" t="s">
+      <c r="D236" s="1" t="s">
         <v>1488</v>
-      </c>
-      <c r="C236" s="4" t="s">
-        <v>1489</v>
-      </c>
-      <c r="D236" s="1" t="s">
-        <v>1490</v>
       </c>
       <c r="E236" s="1">
         <v>1668259.0</v>
       </c>
       <c r="F236" s="1" t="s">
+        <v>1489</v>
+      </c>
+      <c r="G236" s="1" t="s">
+        <v>1587</v>
+      </c>
+      <c r="H236" s="1" t="s">
         <v>1491</v>
-      </c>
-      <c r="G236" s="1" t="s">
-        <v>1492</v>
-      </c>
-      <c r="H236" s="1" t="s">
-        <v>1493</v>
       </c>
       <c r="I236" s="2" t="s">
         <v>1126</v>
@@ -38010,29 +38111,29 @@
         <v>295</v>
       </c>
       <c r="M236" s="2" t="s">
-        <v>1568</v>
+        <v>1588</v>
       </c>
       <c r="N236" s="2" t="s">
-        <v>1569</v>
+        <v>1589</v>
       </c>
       <c r="O236" s="2" t="s">
-        <v>1570</v>
+        <v>1590</v>
       </c>
       <c r="P236" s="2" t="s">
-        <v>1571</v>
+        <v>1591</v>
       </c>
       <c r="Q236" s="2" t="s">
-        <v>1572</v>
+        <v>1592</v>
       </c>
       <c r="R236" s="2" t="s">
-        <v>1573</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="7"/>
       <c r="B237" s="7"/>
       <c r="C237" s="4" t="s">
-        <v>1574</v>
+        <v>1594</v>
       </c>
       <c r="D237" s="7"/>
       <c r="E237" s="7"/>
@@ -38046,28 +38147,28 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>1494</v>
+        <v>1497</v>
       </c>
       <c r="B238" s="15" t="s">
-        <v>1495</v>
+        <v>1498</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>1496</v>
+        <v>1499</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>1497</v>
+        <v>1500</v>
       </c>
       <c r="E238" s="1">
         <v>2700.0</v>
       </c>
       <c r="F238" s="1" t="s">
-        <v>1498</v>
+        <v>1501</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>1499</v>
+        <v>1502</v>
       </c>
       <c r="H238" s="1" t="s">
-        <v>1500</v>
+        <v>1503</v>
       </c>
       <c r="I238" s="1" t="s">
         <v>25</v>
@@ -38082,29 +38183,29 @@
         <v>25</v>
       </c>
       <c r="M238" s="2" t="s">
-        <v>1501</v>
+        <v>1504</v>
       </c>
       <c r="N238" s="2" t="s">
-        <v>1502</v>
+        <v>1505</v>
       </c>
       <c r="O238" s="2" t="s">
-        <v>1503</v>
+        <v>1506</v>
       </c>
       <c r="P238" s="2" t="s">
         <v>127</v>
       </c>
       <c r="Q238" s="2" t="s">
-        <v>1504</v>
+        <v>1507</v>
       </c>
       <c r="R238" s="2" t="s">
-        <v>1505</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1"/>
       <c r="B239" s="15"/>
       <c r="C239" s="4" t="s">
-        <v>1506</v>
+        <v>1509</v>
       </c>
       <c r="D239" s="7"/>
       <c r="E239" s="7"/>
@@ -38118,28 +38219,28 @@
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>1507</v>
+        <v>1510</v>
       </c>
       <c r="B240" s="15" t="s">
-        <v>1508</v>
+        <v>1511</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>1509</v>
+        <v>1512</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>1510</v>
+        <v>1513</v>
       </c>
       <c r="E240" s="1">
         <v>1855.0</v>
       </c>
       <c r="F240" s="1" t="s">
-        <v>1511</v>
+        <v>1514</v>
       </c>
       <c r="G240" s="1" t="s">
-        <v>1512</v>
+        <v>1515</v>
       </c>
       <c r="H240" s="1" t="s">
-        <v>1513</v>
+        <v>1595</v>
       </c>
       <c r="I240" s="1" t="s">
         <v>60</v>
@@ -38154,48 +38255,48 @@
         <v>25</v>
       </c>
       <c r="M240" s="2" t="s">
-        <v>1514</v>
+        <v>1517</v>
       </c>
       <c r="N240" s="2" t="s">
-        <v>1515</v>
+        <v>1518</v>
       </c>
       <c r="O240" s="2" t="s">
-        <v>1516</v>
+        <v>1519</v>
       </c>
       <c r="P240" s="2" t="s">
-        <v>1517</v>
+        <v>1520</v>
       </c>
       <c r="Q240" s="2" t="s">
-        <v>1518</v>
+        <v>1521</v>
       </c>
       <c r="R240" s="2" t="s">
-        <v>1519</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="s">
-        <v>1520</v>
+        <v>1523</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>1521</v>
+        <v>1524</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>1522</v>
+        <v>1525</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>1523</v>
+        <v>1526</v>
       </c>
       <c r="E241" s="1">
         <v>43831.0</v>
       </c>
       <c r="F241" s="1" t="s">
-        <v>1524</v>
+        <v>1527</v>
       </c>
       <c r="G241" s="1" t="s">
-        <v>1525</v>
+        <v>1528</v>
       </c>
       <c r="H241" s="1" t="s">
-        <v>1526</v>
+        <v>1529</v>
       </c>
       <c r="I241" s="1" t="s">
         <v>707</v>
@@ -38210,51 +38311,51 @@
         <v>25</v>
       </c>
       <c r="M241" s="2" t="s">
-        <v>1527</v>
+        <v>1530</v>
       </c>
       <c r="N241" s="2" t="s">
-        <v>1528</v>
+        <v>1531</v>
       </c>
       <c r="O241" s="2" t="s">
-        <v>1529</v>
+        <v>1532</v>
       </c>
       <c r="P241" s="2" t="s">
-        <v>1530</v>
+        <v>1533</v>
       </c>
       <c r="Q241" s="2" t="s">
-        <v>1531</v>
+        <v>1534</v>
       </c>
       <c r="R241" s="2" t="s">
-        <v>1532</v>
+        <v>1535</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="s">
-        <v>1533</v>
+        <v>1536</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>1534</v>
+        <v>1537</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>1535</v>
+        <v>1538</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>1536</v>
+        <v>1539</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>1537</v>
+        <v>1540</v>
       </c>
       <c r="F242" s="1" t="s">
-        <v>1538</v>
+        <v>1541</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>1539</v>
+        <v>1542</v>
       </c>
       <c r="H242" s="1" t="s">
-        <v>1540</v>
+        <v>1543</v>
       </c>
       <c r="I242" s="1" t="s">
-        <v>1541</v>
+        <v>1544</v>
       </c>
       <c r="J242" s="1" t="s">
         <v>25</v>
@@ -38269,19 +38370,19 @@
         <v>1450</v>
       </c>
       <c r="N242" s="2" t="s">
-        <v>1542</v>
+        <v>1545</v>
       </c>
       <c r="O242" s="2" t="s">
-        <v>1543</v>
+        <v>1546</v>
       </c>
       <c r="P242" s="2" t="s">
-        <v>1544</v>
+        <v>1547</v>
       </c>
       <c r="Q242" s="2" t="s">
-        <v>1545</v>
+        <v>1548</v>
       </c>
       <c r="R242" s="2" t="s">
-        <v>1546</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="243">
@@ -38289,7 +38390,7 @@
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
       <c r="D243" s="1" t="s">
-        <v>1547</v>
+        <v>1550</v>
       </c>
       <c r="E243" s="1"/>
       <c r="F243" s="1"/>
@@ -38302,31 +38403,31 @@
     </row>
     <row r="244">
       <c r="A244" s="1" t="s">
-        <v>1548</v>
+        <v>1551</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>1549</v>
+        <v>1552</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>1550</v>
+        <v>1553</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>1551</v>
+        <v>1554</v>
       </c>
       <c r="E244" s="1" t="s">
-        <v>1552</v>
+        <v>1555</v>
       </c>
       <c r="F244" s="1" t="s">
-        <v>1553</v>
+        <v>1556</v>
       </c>
       <c r="G244" s="1" t="s">
-        <v>1554</v>
+        <v>1557</v>
       </c>
       <c r="H244" s="1" t="s">
-        <v>1555</v>
+        <v>1558</v>
       </c>
       <c r="I244" s="1" t="s">
-        <v>1556</v>
+        <v>1559</v>
       </c>
       <c r="J244" s="1" t="s">
         <v>25</v>
@@ -38338,22 +38439,22 @@
         <v>25</v>
       </c>
       <c r="M244" s="2" t="s">
-        <v>1557</v>
+        <v>1560</v>
       </c>
       <c r="N244" s="2" t="s">
-        <v>1558</v>
+        <v>1561</v>
       </c>
       <c r="O244" s="2" t="s">
-        <v>1559</v>
+        <v>1562</v>
       </c>
       <c r="P244" s="2" t="s">
-        <v>1560</v>
+        <v>1563</v>
       </c>
       <c r="Q244" s="2" t="s">
-        <v>1561</v>
+        <v>1564</v>
       </c>
       <c r="R244" s="2" t="s">
-        <v>1562</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="245">
@@ -38361,7 +38462,7 @@
       <c r="B245" s="8"/>
       <c r="C245" s="8"/>
       <c r="D245" s="8" t="s">
-        <v>1563</v>
+        <v>1566</v>
       </c>
       <c r="E245" s="8"/>
       <c r="F245" s="8"/>
@@ -51057,13 +51158,13 @@
     </row>
     <row r="165">
       <c r="A165" s="2" t="s">
-        <v>1575</v>
+        <v>1596</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>1575</v>
+        <v>1596</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>1575</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="167">
@@ -51354,24 +51455,24 @@
     </row>
     <row r="231">
       <c r="A231" s="2" t="s">
-        <v>1465</v>
+        <v>1585</v>
       </c>
       <c r="F231" s="2" t="s">
-        <v>1465</v>
+        <v>1585</v>
       </c>
       <c r="G231" s="2" t="s">
-        <v>1465</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="2" t="s">
-        <v>1465</v>
+        <v>1585</v>
       </c>
       <c r="F233" s="2" t="s">
-        <v>1465</v>
+        <v>1585</v>
       </c>
       <c r="G233" s="2" t="s">
-        <v>1465</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="234">
@@ -51398,24 +51499,24 @@
     </row>
     <row r="240">
       <c r="A240" s="2" t="s">
-        <v>1541</v>
+        <v>1544</v>
       </c>
       <c r="F240" s="2" t="s">
-        <v>1541</v>
+        <v>1544</v>
       </c>
       <c r="G240" s="2" t="s">
-        <v>1541</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="2" t="s">
-        <v>1556</v>
+        <v>1559</v>
       </c>
       <c r="F242" s="2" t="s">
-        <v>1556</v>
+        <v>1559</v>
       </c>
       <c r="G242" s="2" t="s">
-        <v>1556</v>
+        <v>1559</v>
       </c>
     </row>
   </sheetData>
@@ -51453,7 +51554,7 @@
         <v>1.0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1576</v>
+        <v>1597</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -51463,7 +51564,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1577</v>
+        <v>1598</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -51522,7 +51623,7 @@
         <v>4474.0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>1578</v>
+        <v>1599</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>22</v>
@@ -51531,10 +51632,10 @@
         <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>1579</v>
+        <v>1600</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>25</v>
@@ -51543,7 +51644,7 @@
         <v>26</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>27</v>
@@ -51555,7 +51656,7 @@
         <v>29</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>1581</v>
+        <v>1602</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>31</v>
@@ -51635,19 +51736,19 @@
         <v>48659.0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1582</v>
+        <v>1603</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1583</v>
+        <v>1604</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>41</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>1584</v>
+        <v>1605</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>25</v>
@@ -51739,13 +51840,13 @@
         <v>55</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1585</v>
+        <v>1606</v>
       </c>
       <c r="E8" s="1">
         <v>1378.0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1586</v>
+        <v>1607</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>57</v>
@@ -51754,7 +51855,7 @@
         <v>58</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>1587</v>
+        <v>1608</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>60</v>
@@ -51766,7 +51867,7 @@
         <v>61</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N8" s="2" t="s">
         <v>62</v>
@@ -51819,20 +51920,20 @@
       <c r="E10" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="25" t="s">
-        <v>1588</v>
-      </c>
-      <c r="G10" s="25" t="s">
+      <c r="F10" s="26" t="s">
+        <v>1609</v>
+      </c>
+      <c r="G10" s="26" t="s">
         <v>75</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>76</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>1589</v>
+        <v>1610</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>44</v>
@@ -51841,7 +51942,7 @@
         <v>26</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>1590</v>
+        <v>1611</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>78</v>
@@ -51853,7 +51954,7 @@
         <v>80</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>1591</v>
+        <v>1612</v>
       </c>
       <c r="R10" s="2" t="s">
         <v>82</v>
@@ -51913,7 +52014,7 @@
         <v>53301.0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1592</v>
+        <v>1613</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>90</v>
@@ -51922,10 +52023,10 @@
         <v>91</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>1593</v>
+        <v>1614</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>44</v>
@@ -51934,7 +52035,7 @@
         <v>26</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>93</v>
@@ -52008,19 +52109,19 @@
         <v>26682.0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1594</v>
+        <v>1615</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>106</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>1595</v>
+        <v>1616</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>108</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>25</v>
@@ -52041,7 +52142,7 @@
         <v>111</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>1596</v>
+        <v>1617</v>
       </c>
       <c r="R16" s="2" t="s">
         <v>113</v>
@@ -52101,19 +52202,19 @@
         <v>4873.0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1597</v>
+        <v>1618</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>121</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>1598</v>
+        <v>1619</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>1599</v>
+        <v>1620</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>44</v>
@@ -52122,7 +52223,7 @@
         <v>43</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>124</v>
@@ -52134,7 +52235,7 @@
         <v>126</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>1600</v>
+        <v>1621</v>
       </c>
       <c r="R19" s="2" t="s">
         <v>128</v>
@@ -52194,7 +52295,7 @@
         <v>136</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1601</v>
+        <v>1622</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>137</v>
@@ -52206,7 +52307,7 @@
         <v>139</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>44</v>
@@ -52215,7 +52316,7 @@
         <v>26</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>140</v>
@@ -52227,7 +52328,7 @@
         <v>142</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>1602</v>
+        <v>1623</v>
       </c>
       <c r="R22" s="2" t="s">
         <v>144</v>
@@ -52270,19 +52371,19 @@
         <v>189133.0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>1603</v>
+        <v>1624</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>1604</v>
+        <v>1625</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>1605</v>
+        <v>1626</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>1606</v>
+        <v>1627</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>1607</v>
+        <v>1628</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>25</v>
@@ -52291,7 +52392,7 @@
         <v>61</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>155</v>
@@ -52303,7 +52404,7 @@
         <v>157</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>1608</v>
+        <v>1629</v>
       </c>
       <c r="R24" s="2" t="s">
         <v>159</v>
@@ -52348,7 +52449,7 @@
         <v>167</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>1609</v>
+        <v>1630</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>168</v>
@@ -52360,7 +52461,7 @@
         <v>170</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>1610</v>
+        <v>1631</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>172</v>
@@ -52369,7 +52470,7 @@
         <v>26</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N26" s="2" t="s">
         <v>173</v>
@@ -52381,7 +52482,7 @@
         <v>175</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>1611</v>
+        <v>1632</v>
       </c>
       <c r="R26" s="2" t="s">
         <v>177</v>
@@ -52422,7 +52523,7 @@
         <v>183</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1612</v>
+        <v>1633</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>184</v>
@@ -52434,7 +52535,7 @@
         <v>186</v>
       </c>
       <c r="J28" s="14" t="s">
-        <v>1613</v>
+        <v>1634</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>44</v>
@@ -52443,7 +52544,7 @@
         <v>26</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>188</v>
@@ -52517,19 +52618,19 @@
         <v>946.0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>1614</v>
+        <v>1635</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>202</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>1615</v>
+        <v>1636</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>204</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>25</v>
@@ -52538,7 +52639,7 @@
         <v>205</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N31" s="2" t="s">
         <v>45</v>
@@ -52650,7 +52751,7 @@
         <v>802.0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1616</v>
+        <v>1637</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>221</v>
@@ -52671,7 +52772,7 @@
         <v>205</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N36" s="2" t="s">
         <v>93</v>
@@ -52746,7 +52847,7 @@
         <v>236</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>1617</v>
+        <v>1638</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>237</v>
@@ -52755,10 +52856,10 @@
         <v>238</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>239</v>
+        <v>1569</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>1618</v>
+        <v>1639</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>44</v>
@@ -52767,7 +52868,7 @@
         <v>26</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N39" s="2" t="s">
         <v>241</v>
@@ -52841,16 +52942,16 @@
         <v>589.0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>1619</v>
+        <v>1640</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>254</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>1620</v>
+        <v>1641</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>1621</v>
+        <v>1642</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>60</v>
@@ -52862,7 +52963,7 @@
         <v>43</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N42" s="2" t="s">
         <v>257</v>
@@ -52890,7 +52991,7 @@
         <v>263</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>1622</v>
+        <v>1643</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
@@ -52938,19 +53039,19 @@
         <v>12904.0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>1623</v>
+        <v>1644</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>1624</v>
+        <v>1645</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>272</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>1625</v>
+        <v>1646</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>1626</v>
+        <v>1647</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>275</v>
@@ -52959,7 +53060,7 @@
         <v>61</v>
       </c>
       <c r="M45" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>276</v>
@@ -53093,19 +53194,19 @@
         <v>290</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>1627</v>
+        <v>1648</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>291</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>1628</v>
+        <v>1649</v>
       </c>
       <c r="I52" s="1" t="s">
         <v>293</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>1629</v>
+        <v>1650</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>295</v>
@@ -53114,7 +53215,7 @@
         <v>43</v>
       </c>
       <c r="M52" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N52" s="2" t="s">
         <v>296</v>
@@ -53203,19 +53304,19 @@
         <v>309</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>1630</v>
+        <v>1651</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>310</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>1631</v>
+        <v>1652</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>1632</v>
+        <v>1653</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>1633</v>
+        <v>1654</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>25</v>
@@ -53224,19 +53325,19 @@
         <v>26</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N56" s="2" t="s">
-        <v>1634</v>
+        <v>1655</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>1635</v>
+        <v>1656</v>
       </c>
       <c r="P56" s="2" t="s">
-        <v>1636</v>
+        <v>1657</v>
       </c>
       <c r="Q56" s="2" t="s">
-        <v>1637</v>
+        <v>1658</v>
       </c>
       <c r="R56" s="2" t="s">
         <v>318</v>
@@ -53296,7 +53397,7 @@
         <v>1909.0</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>1638</v>
+        <v>1659</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>326</v>
@@ -53305,10 +53406,10 @@
         <v>327</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>1639</v>
+        <v>1660</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>329</v>
@@ -53317,7 +53418,7 @@
         <v>43</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>330</v>
@@ -53372,16 +53473,16 @@
         <v>340</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>1640</v>
+        <v>1661</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>1641</v>
+        <v>1662</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>342</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>1642</v>
+        <v>1663</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>344</v>
@@ -53393,7 +53494,7 @@
         <v>43</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N61" s="2" t="s">
         <v>345</v>
@@ -53467,7 +53568,7 @@
         <v>358</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>1643</v>
+        <v>1664</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>359</v>
@@ -53476,10 +53577,10 @@
         <v>360</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>1644</v>
+        <v>1665</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>25</v>
@@ -53488,16 +53589,16 @@
         <v>26</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N64" s="2" t="s">
         <v>362</v>
       </c>
       <c r="O64" s="2" t="s">
-        <v>1645</v>
+        <v>1666</v>
       </c>
       <c r="P64" s="2" t="s">
-        <v>1646</v>
+        <v>1667</v>
       </c>
       <c r="Q64" s="2" t="s">
         <v>365</v>
@@ -53526,7 +53627,7 @@
         <v>373</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>1647</v>
+        <v>1668</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>374</v>
@@ -53538,7 +53639,7 @@
         <v>376</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>25</v>
@@ -53547,7 +53648,7 @@
         <v>26</v>
       </c>
       <c r="M65" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N65" s="15" t="s">
         <v>377</v>
@@ -53617,7 +53718,7 @@
         <v>388</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>1648</v>
+        <v>1669</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>389</v>
@@ -53626,10 +53727,10 @@
         <v>390</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>1649</v>
+        <v>1670</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>1650</v>
+        <v>1671</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>44</v>
@@ -53638,7 +53739,7 @@
         <v>26</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N68" s="2" t="s">
         <v>393</v>
@@ -53650,7 +53751,7 @@
         <v>395</v>
       </c>
       <c r="Q68" s="2" t="s">
-        <v>1651</v>
+        <v>1672</v>
       </c>
       <c r="R68" s="2" t="s">
         <v>397</v>
@@ -53691,7 +53792,7 @@
         <v>1724839.0</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>1652</v>
+        <v>1673</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>403</v>
@@ -53700,10 +53801,10 @@
         <v>404</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>1653</v>
+        <v>1674</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>1654</v>
+        <v>1675</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>25</v>
@@ -53712,16 +53813,16 @@
         <v>26</v>
       </c>
       <c r="M70" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N70" s="2" t="s">
         <v>406</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>1655</v>
+        <v>1676</v>
       </c>
       <c r="P70" s="2" t="s">
-        <v>1656</v>
+        <v>1677</v>
       </c>
       <c r="Q70" s="2" t="s">
         <v>409</v>
@@ -53767,19 +53868,19 @@
         <v>47525.0</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>1657</v>
+        <v>1678</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>417</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>1658</v>
+        <v>1679</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>1659</v>
+        <v>1680</v>
       </c>
       <c r="J72" s="2" t="s">
-        <v>1660</v>
+        <v>1681</v>
       </c>
       <c r="K72" s="1" t="s">
         <v>25</v>
@@ -53788,7 +53889,7 @@
         <v>43</v>
       </c>
       <c r="M72" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N72" s="2" t="s">
         <v>421</v>
@@ -53816,7 +53917,7 @@
         <v>427</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>428</v>
+        <v>1571</v>
       </c>
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
@@ -53862,19 +53963,19 @@
         <v>779.0</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>1661</v>
+        <v>1682</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>1662</v>
+        <v>1683</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>435</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>1663</v>
+        <v>1684</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>1664</v>
+        <v>1685</v>
       </c>
       <c r="K75" s="1" t="s">
         <v>44</v>
@@ -53883,7 +53984,7 @@
         <v>61</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N75" s="2" t="s">
         <v>438</v>
@@ -53892,10 +53993,10 @@
         <v>439</v>
       </c>
       <c r="P75" s="2" t="s">
-        <v>1665</v>
+        <v>1686</v>
       </c>
       <c r="Q75" s="2" t="s">
-        <v>1666</v>
+        <v>1687</v>
       </c>
       <c r="R75" s="2" t="s">
         <v>442</v>
@@ -53938,19 +54039,19 @@
         <v>3671.0</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1667</v>
+        <v>1688</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>1668</v>
+        <v>1689</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>450</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>1669</v>
+        <v>1690</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K77" s="1" t="s">
         <v>44</v>
@@ -53959,7 +54060,7 @@
         <v>205</v>
       </c>
       <c r="M77" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N77" s="2" t="s">
         <v>452</v>
@@ -53971,7 +54072,7 @@
         <v>454</v>
       </c>
       <c r="Q77" s="2" t="s">
-        <v>1670</v>
+        <v>1691</v>
       </c>
       <c r="R77" s="2" t="s">
         <v>456</v>
@@ -54012,19 +54113,19 @@
         <v>462</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>1671</v>
+        <v>1692</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>463</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>1672</v>
+        <v>1693</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>1673</v>
+        <v>1694</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>1674</v>
+        <v>1695</v>
       </c>
       <c r="K79" s="1" t="s">
         <v>25</v>
@@ -54033,7 +54134,7 @@
         <v>43</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N79" s="2" t="s">
         <v>467</v>
@@ -54045,7 +54146,7 @@
         <v>469</v>
       </c>
       <c r="Q79" s="2" t="s">
-        <v>1675</v>
+        <v>1696</v>
       </c>
       <c r="R79" s="2" t="s">
         <v>471</v>
@@ -54095,7 +54196,7 @@
       <c r="B82" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="C82" s="21" t="s">
+      <c r="C82" s="22" t="s">
         <v>477</v>
       </c>
       <c r="D82" s="1" t="s">
@@ -54105,19 +54206,19 @@
         <v>766.0</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>1676</v>
+        <v>1697</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>1677</v>
+        <v>1698</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>480</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>1678</v>
+        <v>1699</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>1679</v>
+        <v>1700</v>
       </c>
       <c r="K82" s="1" t="s">
         <v>44</v>
@@ -54126,7 +54227,7 @@
         <v>43</v>
       </c>
       <c r="M82" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N82" s="2" t="s">
         <v>483</v>
@@ -54138,7 +54239,7 @@
         <v>485</v>
       </c>
       <c r="Q82" s="2" t="s">
-        <v>1680</v>
+        <v>1701</v>
       </c>
       <c r="R82" s="2" t="s">
         <v>487</v>
@@ -54198,19 +54299,19 @@
         <v>495</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>1681</v>
+        <v>1702</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>1682</v>
+        <v>1703</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>1683</v>
+        <v>1704</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>1684</v>
+        <v>1705</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>1685</v>
+        <v>1706</v>
       </c>
       <c r="K85" s="1" t="s">
         <v>25</v>
@@ -54219,7 +54320,7 @@
         <v>500</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N85" s="2" t="s">
         <v>501</v>
@@ -54231,7 +54332,7 @@
         <v>503</v>
       </c>
       <c r="Q85" s="2" t="s">
-        <v>1686</v>
+        <v>1707</v>
       </c>
       <c r="R85" s="2" t="s">
         <v>505</v>
@@ -54272,7 +54373,7 @@
         <v>8229.0</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>1687</v>
+        <v>1708</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>511</v>
@@ -54281,10 +54382,10 @@
         <v>512</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>1688</v>
+        <v>1709</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>1689</v>
+        <v>1710</v>
       </c>
       <c r="K87" s="1" t="s">
         <v>44</v>
@@ -54293,7 +54394,7 @@
         <v>515</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N87" s="2" t="s">
         <v>516</v>
@@ -54331,7 +54432,7 @@
         <v>1590.0</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>1690</v>
+        <v>1711</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>526</v>
@@ -54340,10 +54441,10 @@
         <v>527</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>1691</v>
+        <v>1712</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>1692</v>
+        <v>1713</v>
       </c>
       <c r="K88" s="1" t="s">
         <v>44</v>
@@ -54352,19 +54453,19 @@
         <v>205</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>1564</v>
+        <v>1572</v>
       </c>
       <c r="O88" s="2" t="s">
-        <v>1565</v>
+        <v>1573</v>
       </c>
       <c r="P88" s="2" t="s">
-        <v>1566</v>
+        <v>1574</v>
       </c>
       <c r="Q88" s="2" t="s">
-        <v>1693</v>
+        <v>1714</v>
       </c>
       <c r="R88" s="2" t="s">
         <v>534</v>
@@ -54391,7 +54492,7 @@
       <c r="M89" s="7"/>
     </row>
     <row r="90">
-      <c r="A90" s="22" t="s">
+      <c r="A90" s="23" t="s">
         <v>538</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -54407,19 +54508,19 @@
         <v>542</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>1694</v>
+        <v>1715</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>1695</v>
+        <v>1716</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>544</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>1696</v>
+        <v>1717</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>1697</v>
+        <v>1718</v>
       </c>
       <c r="K90" s="1" t="s">
         <v>25</v>
@@ -54428,7 +54529,7 @@
         <v>43</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N90" s="2" t="s">
         <v>547</v>
@@ -54450,7 +54551,7 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="22"/>
+      <c r="A91" s="23"/>
       <c r="B91" s="1"/>
       <c r="C91" s="4" t="s">
         <v>553</v>
@@ -54469,7 +54570,7 @@
       <c r="M91" s="7"/>
     </row>
     <row r="92">
-      <c r="A92" s="22"/>
+      <c r="A92" s="23"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="15" t="s">
@@ -54502,19 +54603,19 @@
         <v>1228.0</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>1698</v>
+        <v>1719</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>560</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>1699</v>
+        <v>1720</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>1700</v>
+        <v>1721</v>
       </c>
       <c r="J93" s="2" t="s">
-        <v>1701</v>
+        <v>1722</v>
       </c>
       <c r="K93" s="1" t="s">
         <v>25</v>
@@ -54523,7 +54624,7 @@
         <v>205</v>
       </c>
       <c r="M93" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N93" s="2" t="s">
         <v>564</v>
@@ -54535,7 +54636,7 @@
         <v>566</v>
       </c>
       <c r="Q93" s="15" t="s">
-        <v>1702</v>
+        <v>1723</v>
       </c>
       <c r="R93" s="2" t="s">
         <v>568</v>
@@ -54579,19 +54680,19 @@
         <v>9883.0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>1703</v>
+        <v>1724</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>576</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>1704</v>
+        <v>1725</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>1705</v>
+        <v>1726</v>
       </c>
       <c r="J95" s="1" t="s">
-        <v>1706</v>
+        <v>1727</v>
       </c>
       <c r="K95" s="1" t="s">
         <v>25</v>
@@ -54600,7 +54701,7 @@
         <v>43</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N95" s="2" t="s">
         <v>580</v>
@@ -54669,7 +54770,7 @@
         <v>420.0</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>1707</v>
+        <v>1728</v>
       </c>
       <c r="G98" s="1" t="s">
         <v>591</v>
@@ -54678,7 +54779,7 @@
         <v>592</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>1708</v>
+        <v>1729</v>
       </c>
       <c r="J98" s="1" t="s">
         <v>60</v>
@@ -54690,7 +54791,7 @@
         <v>43</v>
       </c>
       <c r="M98" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N98" s="2" t="s">
         <v>594</v>
@@ -54745,7 +54846,7 @@
         <v>1927.0</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>1709</v>
+        <v>1730</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>605</v>
@@ -54754,7 +54855,7 @@
         <v>606</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>1710</v>
+        <v>1731</v>
       </c>
       <c r="J100" s="1" t="s">
         <v>60</v>
@@ -54766,7 +54867,7 @@
         <v>205</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N100" s="2" t="s">
         <v>608</v>
@@ -54778,7 +54879,7 @@
         <v>610</v>
       </c>
       <c r="Q100" s="2" t="s">
-        <v>1711</v>
+        <v>1732</v>
       </c>
       <c r="R100" s="2" t="s">
         <v>612</v>
@@ -54809,7 +54910,7 @@
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1" t="s">
-        <v>1712</v>
+        <v>1733</v>
       </c>
       <c r="E102" s="1"/>
       <c r="F102" s="7"/>
@@ -54838,19 +54939,19 @@
         <v>2303.0</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>1713</v>
+        <v>1734</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>620</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>1714</v>
+        <v>1735</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>622</v>
       </c>
       <c r="J103" s="1" t="s">
-        <v>1715</v>
+        <v>1736</v>
       </c>
       <c r="K103" s="1" t="s">
         <v>44</v>
@@ -54859,7 +54960,7 @@
         <v>43</v>
       </c>
       <c r="M103" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N103" s="2" t="s">
         <v>438</v>
@@ -54897,7 +54998,7 @@
         <v>8813.0</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>1716</v>
+        <v>1737</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>633</v>
@@ -54906,10 +55007,10 @@
         <v>634</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>1717</v>
+        <v>1738</v>
       </c>
       <c r="J104" s="1" t="s">
-        <v>1718</v>
+        <v>1739</v>
       </c>
       <c r="K104" s="1" t="s">
         <v>25</v>
@@ -54918,7 +55019,7 @@
         <v>43</v>
       </c>
       <c r="M104" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N104" s="2" t="s">
         <v>637</v>
@@ -54930,7 +55031,7 @@
         <v>639</v>
       </c>
       <c r="Q104" s="2" t="s">
-        <v>1719</v>
+        <v>1740</v>
       </c>
       <c r="R104" s="2" t="s">
         <v>641</v>
@@ -54956,19 +55057,19 @@
         <v>55505.0</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>1720</v>
+        <v>1741</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>1721</v>
+        <v>1742</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>648</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>1722</v>
+        <v>1743</v>
       </c>
       <c r="J105" s="1" t="s">
-        <v>1692</v>
+        <v>1713</v>
       </c>
       <c r="K105" s="1" t="s">
         <v>25</v>
@@ -54977,7 +55078,7 @@
         <v>205</v>
       </c>
       <c r="M105" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N105" s="2" t="s">
         <v>650</v>
@@ -54986,7 +55087,7 @@
         <v>651</v>
       </c>
       <c r="P105" s="2" t="s">
-        <v>1723</v>
+        <v>1744</v>
       </c>
     </row>
     <row r="106">
@@ -55023,7 +55124,7 @@
         <v>661</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>1724</v>
+        <v>1745</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>662</v>
@@ -55035,7 +55136,7 @@
         <v>664</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>1692</v>
+        <v>1713</v>
       </c>
       <c r="K107" s="1" t="s">
         <v>44</v>
@@ -55044,7 +55145,7 @@
         <v>205</v>
       </c>
       <c r="M107" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N107" s="2" t="s">
         <v>665</v>
@@ -55090,19 +55191,19 @@
         <v>4044.0</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>1725</v>
+        <v>1746</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>676</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>1726</v>
+        <v>1747</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>1727</v>
+        <v>1748</v>
       </c>
       <c r="J109" s="1" t="s">
-        <v>1701</v>
+        <v>1722</v>
       </c>
       <c r="K109" s="1" t="s">
         <v>44</v>
@@ -55111,7 +55212,7 @@
         <v>205</v>
       </c>
       <c r="M109" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N109" s="2" t="s">
         <v>679</v>
@@ -55155,19 +55256,19 @@
         <v>689</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>1728</v>
+        <v>1749</v>
       </c>
       <c r="G111" s="1" t="s">
         <v>690</v>
       </c>
       <c r="H111" s="15" t="s">
-        <v>1729</v>
+        <v>1750</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>692</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>1730</v>
+        <v>1751</v>
       </c>
       <c r="K111" s="1" t="s">
         <v>25</v>
@@ -55176,7 +55277,7 @@
         <v>43</v>
       </c>
       <c r="M111" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N111" s="2" t="s">
         <v>693</v>
@@ -55222,19 +55323,19 @@
         <v>58288.0</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>1731</v>
+        <v>1752</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>704</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>1732</v>
+        <v>1753</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>706</v>
       </c>
       <c r="J113" s="1" t="s">
-        <v>1733</v>
+        <v>1754</v>
       </c>
       <c r="K113" s="1" t="s">
         <v>25</v>
@@ -55243,16 +55344,16 @@
         <v>26</v>
       </c>
       <c r="M113" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N113" s="2" t="s">
         <v>608</v>
       </c>
       <c r="O113" s="2" t="s">
-        <v>1734</v>
+        <v>1755</v>
       </c>
       <c r="P113" s="2" t="s">
-        <v>1735</v>
+        <v>1756</v>
       </c>
     </row>
     <row r="114">
@@ -55287,19 +55388,19 @@
         <v>718</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>1736</v>
+        <v>1757</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>719</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>1737</v>
+        <v>1758</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>721</v>
       </c>
       <c r="J115" s="1" t="s">
-        <v>1738</v>
+        <v>1759</v>
       </c>
       <c r="K115" s="1" t="s">
         <v>25</v>
@@ -55308,7 +55409,7 @@
         <v>43</v>
       </c>
       <c r="M115" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N115" s="2" t="s">
         <v>723</v>
@@ -55317,14 +55418,14 @@
         <v>724</v>
       </c>
       <c r="P115" s="2" t="s">
-        <v>1739</v>
+        <v>1760</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
-      <c r="D116" s="24" t="s">
+      <c r="D116" s="25" t="s">
         <v>729</v>
       </c>
       <c r="E116" s="7"/>
@@ -55354,7 +55455,7 @@
         <v>734</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>1740</v>
+        <v>1761</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>735</v>
@@ -55366,7 +55467,7 @@
         <v>737</v>
       </c>
       <c r="J117" s="1" t="s">
-        <v>1741</v>
+        <v>1762</v>
       </c>
       <c r="K117" s="1" t="s">
         <v>25</v>
@@ -55375,7 +55476,7 @@
         <v>43</v>
       </c>
       <c r="M117" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N117" s="2" t="s">
         <v>739</v>
@@ -55384,7 +55485,7 @@
         <v>740</v>
       </c>
       <c r="P117" s="2" t="s">
-        <v>1742</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="118">
@@ -55419,19 +55520,19 @@
         <v>9295.0</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>1743</v>
+        <v>1764</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>749</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>1744</v>
+        <v>1765</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>1745</v>
+        <v>1766</v>
       </c>
       <c r="J119" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K119" s="1" t="s">
         <v>25</v>
@@ -55440,7 +55541,7 @@
         <v>26</v>
       </c>
       <c r="M119" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N119" s="2" t="s">
         <v>752</v>
@@ -55486,7 +55587,7 @@
         <v>78380.0</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>1746</v>
+        <v>1767</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>762</v>
@@ -55507,7 +55608,7 @@
         <v>61</v>
       </c>
       <c r="M121" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N121" s="2" t="s">
         <v>765</v>
@@ -55516,7 +55617,7 @@
         <v>766</v>
       </c>
       <c r="P121" s="2" t="s">
-        <v>1747</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="122">
@@ -55553,19 +55654,19 @@
         <v>1738982.0</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>1748</v>
+        <v>1769</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>776</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>1749</v>
+        <v>1770</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>1750</v>
+        <v>1771</v>
       </c>
       <c r="J123" s="1" t="s">
-        <v>1679</v>
+        <v>1700</v>
       </c>
       <c r="K123" s="1" t="s">
         <v>25</v>
@@ -55574,16 +55675,16 @@
         <v>43</v>
       </c>
       <c r="M123" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N123" s="2" t="s">
         <v>779</v>
       </c>
       <c r="O123" s="2" t="s">
-        <v>1751</v>
+        <v>1772</v>
       </c>
       <c r="P123" s="2" t="s">
-        <v>1752</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="124">
@@ -55620,16 +55721,16 @@
         <v>790</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>1753</v>
+        <v>1774</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>791</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>1754</v>
+        <v>1775</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>1755</v>
+        <v>1776</v>
       </c>
       <c r="J125" s="1" t="s">
         <v>794</v>
@@ -55641,7 +55742,7 @@
         <v>43</v>
       </c>
       <c r="M125" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N125" s="2" t="s">
         <v>795</v>
@@ -55650,7 +55751,7 @@
         <v>796</v>
       </c>
       <c r="P125" s="2" t="s">
-        <v>1756</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="126">
@@ -55740,7 +55841,7 @@
         <v>44885.0</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>1757</v>
+        <v>1778</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>810</v>
@@ -55749,10 +55850,10 @@
         <v>811</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>1758</v>
+        <v>1779</v>
       </c>
       <c r="J130" s="2" t="s">
-        <v>1759</v>
+        <v>1780</v>
       </c>
       <c r="K130" s="1" t="s">
         <v>44</v>
@@ -55761,7 +55862,7 @@
         <v>205</v>
       </c>
       <c r="M130" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N130" s="2" t="s">
         <v>814</v>
@@ -55770,7 +55871,7 @@
         <v>815</v>
       </c>
       <c r="P130" s="2" t="s">
-        <v>1760</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="131">
@@ -55799,25 +55900,25 @@
         <v>822</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>823</v>
+        <v>1576</v>
       </c>
       <c r="E132" s="1">
         <v>16493.0</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>1761</v>
+        <v>1782</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>824</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>1762</v>
+        <v>1783</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>1763</v>
+        <v>1784</v>
       </c>
       <c r="J132" s="1" t="s">
-        <v>1764</v>
+        <v>1785</v>
       </c>
       <c r="K132" s="1" t="s">
         <v>25</v>
@@ -55826,7 +55927,7 @@
         <v>26</v>
       </c>
       <c r="M132" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N132" s="2" t="s">
         <v>828</v>
@@ -55835,7 +55936,7 @@
         <v>829</v>
       </c>
       <c r="P132" s="2" t="s">
-        <v>1765</v>
+        <v>1786</v>
       </c>
     </row>
     <row r="133">
@@ -55870,16 +55971,16 @@
         <v>838</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>1766</v>
+        <v>1787</v>
       </c>
       <c r="G134" s="2" t="s">
         <v>839</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>1767</v>
+        <v>1788</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>1768</v>
+        <v>1789</v>
       </c>
       <c r="J134" s="1" t="s">
         <v>842</v>
@@ -55900,7 +56001,7 @@
         <v>844</v>
       </c>
       <c r="P134" s="2" t="s">
-        <v>1769</v>
+        <v>1790</v>
       </c>
     </row>
     <row r="135">
@@ -55971,7 +56072,7 @@
         <v>856</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>1770</v>
+        <v>1791</v>
       </c>
       <c r="G138" s="1" t="s">
         <v>857</v>
@@ -55983,7 +56084,7 @@
         <v>859</v>
       </c>
       <c r="J138" s="1" t="s">
-        <v>1771</v>
+        <v>1792</v>
       </c>
       <c r="K138" s="1" t="s">
         <v>44</v>
@@ -55992,7 +56093,7 @@
         <v>61</v>
       </c>
       <c r="M138" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N138" s="2" t="s">
         <v>860</v>
@@ -56001,7 +56102,7 @@
         <v>861</v>
       </c>
       <c r="P138" s="2" t="s">
-        <v>1772</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="139">
@@ -56036,7 +56137,7 @@
         <v>870</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>1773</v>
+        <v>1794</v>
       </c>
       <c r="G140" s="1" t="s">
         <v>871</v>
@@ -56045,10 +56146,10 @@
         <v>872</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>1774</v>
+        <v>1795</v>
       </c>
       <c r="J140" s="1" t="s">
-        <v>1775</v>
+        <v>1796</v>
       </c>
       <c r="K140" s="1" t="s">
         <v>25</v>
@@ -56057,7 +56158,7 @@
         <v>61</v>
       </c>
       <c r="M140" s="1" t="s">
-        <v>1776</v>
+        <v>1797</v>
       </c>
       <c r="N140" s="2" t="s">
         <v>875</v>
@@ -56104,7 +56205,7 @@
         <v>9420.0</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>1777</v>
+        <v>1798</v>
       </c>
       <c r="G142" s="1" t="s">
         <v>887</v>
@@ -56113,7 +56214,7 @@
         <v>888</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>1778</v>
+        <v>1799</v>
       </c>
       <c r="J142" s="1" t="s">
         <v>60</v>
@@ -56125,7 +56226,7 @@
         <v>205</v>
       </c>
       <c r="M142" s="1" t="s">
-        <v>1776</v>
+        <v>1797</v>
       </c>
       <c r="N142" s="2" t="s">
         <v>890</v>
@@ -56134,7 +56235,7 @@
         <v>891</v>
       </c>
       <c r="P142" s="2" t="s">
-        <v>1779</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="143">
@@ -56170,19 +56271,19 @@
         <v>901</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>1780</v>
+        <v>1801</v>
       </c>
       <c r="G144" s="1" t="s">
         <v>902</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>1781</v>
+        <v>1802</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>904</v>
       </c>
       <c r="J144" s="1" t="s">
-        <v>1771</v>
+        <v>1792</v>
       </c>
       <c r="K144" s="1" t="s">
         <v>25</v>
@@ -56191,7 +56292,7 @@
         <v>43</v>
       </c>
       <c r="M144" s="1" t="s">
-        <v>1776</v>
+        <v>1797</v>
       </c>
       <c r="N144" s="2" t="s">
         <v>905</v>
@@ -56200,7 +56301,7 @@
         <v>906</v>
       </c>
       <c r="P144" s="2" t="s">
-        <v>1782</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="145">
@@ -56236,19 +56337,19 @@
         <v>916</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>1783</v>
+        <v>1804</v>
       </c>
       <c r="G146" s="1" t="s">
         <v>917</v>
       </c>
       <c r="H146" s="2" t="s">
-        <v>1784</v>
+        <v>1805</v>
       </c>
       <c r="I146" s="2" t="s">
         <v>919</v>
       </c>
       <c r="J146" s="1" t="s">
-        <v>1771</v>
+        <v>1792</v>
       </c>
       <c r="K146" s="1" t="s">
         <v>25</v>
@@ -56257,7 +56358,7 @@
         <v>43</v>
       </c>
       <c r="M146" s="1" t="s">
-        <v>1776</v>
+        <v>1797</v>
       </c>
       <c r="N146" s="2" t="s">
         <v>920</v>
@@ -56266,7 +56367,7 @@
         <v>921</v>
       </c>
       <c r="P146" s="2" t="s">
-        <v>1785</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="147">
@@ -56300,13 +56401,13 @@
         <v>16019.0</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>1786</v>
+        <v>1807</v>
       </c>
       <c r="G148" s="1" t="s">
-        <v>1787</v>
+        <v>1808</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>1788</v>
+        <v>1809</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>932</v>
@@ -56321,7 +56422,7 @@
         <v>205</v>
       </c>
       <c r="M148" s="1" t="s">
-        <v>1776</v>
+        <v>1797</v>
       </c>
       <c r="N148" s="2" t="s">
         <v>933</v>
@@ -56330,7 +56431,7 @@
         <v>934</v>
       </c>
       <c r="P148" s="2" t="s">
-        <v>1789</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="149">
@@ -56366,7 +56467,7 @@
         <v>254931.0</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>1790</v>
+        <v>1811</v>
       </c>
       <c r="G150" s="1" t="s">
         <v>944</v>
@@ -56375,10 +56476,10 @@
         <v>945</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>1791</v>
+        <v>1812</v>
       </c>
       <c r="J150" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K150" s="1" t="s">
         <v>25</v>
@@ -56387,7 +56488,7 @@
         <v>205</v>
       </c>
       <c r="M150" s="1" t="s">
-        <v>1776</v>
+        <v>1797</v>
       </c>
       <c r="N150" s="2" t="s">
         <v>947</v>
@@ -56396,7 +56497,7 @@
         <v>948</v>
       </c>
       <c r="P150" s="2" t="s">
-        <v>1792</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="151">
@@ -56430,16 +56531,16 @@
         <v>25858.0</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>1793</v>
+        <v>1814</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>957</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>1794</v>
+        <v>1815</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>1795</v>
+        <v>1816</v>
       </c>
       <c r="J152" s="1" t="s">
         <v>60</v>
@@ -56451,7 +56552,7 @@
         <v>205</v>
       </c>
       <c r="M152" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N152" s="2" t="s">
         <v>960</v>
@@ -56460,7 +56561,7 @@
         <v>961</v>
       </c>
       <c r="P152" s="2" t="s">
-        <v>1796</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="153">
@@ -56495,19 +56596,19 @@
         <v>970</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>1797</v>
+        <v>1818</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>1798</v>
+        <v>1819</v>
       </c>
       <c r="H154" s="1" t="s">
         <v>972</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>1799</v>
+        <v>1820</v>
       </c>
       <c r="J154" s="1" t="s">
-        <v>1800</v>
+        <v>1821</v>
       </c>
       <c r="K154" s="1" t="s">
         <v>44</v>
@@ -56516,7 +56617,7 @@
         <v>205</v>
       </c>
       <c r="M154" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="N154" s="2" t="s">
         <v>975</v>
@@ -56525,7 +56626,7 @@
         <v>976</v>
       </c>
       <c r="P154" s="2" t="s">
-        <v>1801</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="155">
@@ -56580,7 +56681,7 @@
         <v>43</v>
       </c>
       <c r="M156" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="157">
@@ -56615,7 +56716,7 @@
         <v>38222.0</v>
       </c>
       <c r="F158" s="15" t="s">
-        <v>1802</v>
+        <v>1823</v>
       </c>
       <c r="G158" s="15" t="s">
         <v>1000</v>
@@ -56636,7 +56737,7 @@
         <v>205</v>
       </c>
       <c r="M158" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="159">
@@ -56673,10 +56774,10 @@
         <v>1014</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>1803</v>
+        <v>1824</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>1804</v>
+        <v>1825</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>1016</v>
@@ -56685,7 +56786,7 @@
         <v>1017</v>
       </c>
       <c r="J160" s="1" t="s">
-        <v>1805</v>
+        <v>1826</v>
       </c>
       <c r="K160" s="1" t="s">
         <v>44</v>
@@ -56694,7 +56795,7 @@
         <v>205</v>
       </c>
       <c r="M160" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="161">
@@ -56769,7 +56870,7 @@
         <v>1551.0</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>1806</v>
+        <v>1827</v>
       </c>
       <c r="G164" s="1" t="s">
         <v>1034</v>
@@ -56778,7 +56879,7 @@
         <v>1035</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>1807</v>
+        <v>1828</v>
       </c>
       <c r="J164" s="1" t="s">
         <v>60</v>
@@ -56790,7 +56891,7 @@
         <v>205</v>
       </c>
       <c r="M164" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="165">
@@ -56825,10 +56926,10 @@
         <v>2352.0</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>1808</v>
+        <v>1829</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>1809</v>
+        <v>1830</v>
       </c>
       <c r="H166" s="1" t="s">
         <v>1048</v>
@@ -56837,7 +56938,7 @@
         <v>1049</v>
       </c>
       <c r="J166" s="1" t="s">
-        <v>1810</v>
+        <v>1831</v>
       </c>
       <c r="K166" s="1" t="s">
         <v>25</v>
@@ -56846,7 +56947,7 @@
         <v>43</v>
       </c>
       <c r="M166" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="167">
@@ -56883,13 +56984,13 @@
         <v>1062</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>1811</v>
+        <v>1832</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>1812</v>
+        <v>1833</v>
       </c>
       <c r="H168" s="1" t="s">
-        <v>1813</v>
+        <v>1834</v>
       </c>
       <c r="I168" s="1" t="s">
         <v>1065</v>
@@ -56904,7 +57005,7 @@
         <v>43</v>
       </c>
       <c r="M168" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="169">
@@ -56939,19 +57040,19 @@
         <v>1076</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>1814</v>
+        <v>1835</v>
       </c>
       <c r="G170" s="1" t="s">
         <v>1077</v>
       </c>
       <c r="H170" s="1" t="s">
-        <v>1078</v>
+        <v>1577</v>
       </c>
       <c r="I170" s="1" t="s">
         <v>1079</v>
       </c>
       <c r="J170" s="1" t="s">
-        <v>1815</v>
+        <v>1836</v>
       </c>
       <c r="K170" s="1" t="s">
         <v>25</v>
@@ -56960,7 +57061,7 @@
         <v>1081</v>
       </c>
       <c r="M170" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="171">
@@ -57031,13 +57132,13 @@
         <v>2015.0</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>1816</v>
+        <v>1837</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>1817</v>
+        <v>1838</v>
       </c>
       <c r="H174" s="1" t="s">
-        <v>1818</v>
+        <v>1839</v>
       </c>
       <c r="I174" s="1" t="s">
         <v>1097</v>
@@ -57052,7 +57153,7 @@
         <v>43</v>
       </c>
       <c r="M174" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="175">
@@ -57108,19 +57209,19 @@
         <v>4072.0</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>1819</v>
+        <v>1840</v>
       </c>
       <c r="G177" s="1" t="s">
         <v>1111</v>
       </c>
       <c r="H177" s="1" t="s">
-        <v>1820</v>
+        <v>1841</v>
       </c>
       <c r="I177" s="1" t="s">
-        <v>1821</v>
+        <v>1842</v>
       </c>
       <c r="J177" s="1" t="s">
-        <v>1733</v>
+        <v>1754</v>
       </c>
       <c r="K177" s="1" t="s">
         <v>25</v>
@@ -57129,7 +57230,7 @@
         <v>43</v>
       </c>
       <c r="M177" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="178">
@@ -57164,7 +57265,7 @@
         <v>40921.0</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>1822</v>
+        <v>1843</v>
       </c>
       <c r="G179" s="1"/>
       <c r="H179" s="1" t="s">
@@ -57239,7 +57340,7 @@
         <v>1140</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>1823</v>
+        <v>1844</v>
       </c>
       <c r="G182" s="1" t="s">
         <v>1141</v>
@@ -57248,10 +57349,10 @@
         <v>1142</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>1824</v>
+        <v>1845</v>
       </c>
       <c r="J182" s="1" t="s">
-        <v>1825</v>
+        <v>1846</v>
       </c>
       <c r="K182" s="1" t="s">
         <v>25</v>
@@ -57260,7 +57361,7 @@
         <v>205</v>
       </c>
       <c r="M182" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="183">
@@ -57295,10 +57396,10 @@
         <v>1156</v>
       </c>
       <c r="F184" s="1" t="s">
-        <v>1826</v>
+        <v>1847</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>1827</v>
+        <v>1848</v>
       </c>
       <c r="H184" s="1" t="s">
         <v>1158</v>
@@ -57307,7 +57408,7 @@
         <v>1159</v>
       </c>
       <c r="J184" s="1" t="s">
-        <v>1828</v>
+        <v>1849</v>
       </c>
       <c r="K184" s="1" t="s">
         <v>44</v>
@@ -57316,7 +57417,7 @@
         <v>43</v>
       </c>
       <c r="M184" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="185">
@@ -57389,19 +57490,19 @@
         <v>1175</v>
       </c>
       <c r="F188" s="1" t="s">
-        <v>1829</v>
+        <v>1850</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>1830</v>
+        <v>1851</v>
       </c>
       <c r="H188" s="1" t="s">
-        <v>1831</v>
+        <v>1852</v>
       </c>
       <c r="I188" s="1" t="s">
-        <v>1178</v>
+        <v>1578</v>
       </c>
       <c r="J188" s="1" t="s">
-        <v>1832</v>
+        <v>1853</v>
       </c>
       <c r="K188" s="1" t="s">
         <v>25</v>
@@ -57410,7 +57511,7 @@
         <v>205</v>
       </c>
       <c r="M188" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="189">
@@ -57441,25 +57542,25 @@
         <v>1189</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>1833</v>
+        <v>1854</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>1191</v>
       </c>
       <c r="F190" s="1" t="s">
-        <v>1834</v>
+        <v>1855</v>
       </c>
       <c r="G190" s="1" t="s">
         <v>1192</v>
       </c>
       <c r="H190" s="1" t="s">
-        <v>1835</v>
+        <v>1856</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>1836</v>
+        <v>1857</v>
       </c>
       <c r="J190" s="1" t="s">
-        <v>1837</v>
+        <v>1858</v>
       </c>
       <c r="K190" s="1" t="s">
         <v>44</v>
@@ -57468,7 +57569,7 @@
         <v>43</v>
       </c>
       <c r="M190" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="191">
@@ -57507,19 +57608,19 @@
         <v>1208</v>
       </c>
       <c r="F192" s="1" t="s">
-        <v>1838</v>
+        <v>1859</v>
       </c>
       <c r="G192" s="1" t="s">
         <v>1209</v>
       </c>
       <c r="H192" s="1" t="s">
-        <v>1839</v>
+        <v>1860</v>
       </c>
       <c r="I192" s="1" t="s">
-        <v>1840</v>
+        <v>1861</v>
       </c>
       <c r="J192" s="1" t="s">
-        <v>1841</v>
+        <v>1862</v>
       </c>
       <c r="K192" s="1" t="s">
         <v>25</v>
@@ -57528,7 +57629,7 @@
         <v>26</v>
       </c>
       <c r="M192" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="193">
@@ -57563,19 +57664,19 @@
         <v>1223</v>
       </c>
       <c r="F194" s="1" t="s">
-        <v>1842</v>
+        <v>1863</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>1843</v>
+        <v>1864</v>
       </c>
       <c r="H194" s="1" t="s">
         <v>1225</v>
       </c>
       <c r="I194" s="1" t="s">
-        <v>1844</v>
+        <v>1865</v>
       </c>
       <c r="J194" s="1" t="s">
-        <v>1845</v>
+        <v>1866</v>
       </c>
       <c r="K194" s="1" t="s">
         <v>25</v>
@@ -57584,7 +57685,7 @@
         <v>43</v>
       </c>
       <c r="M194" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="195">
@@ -57640,19 +57741,19 @@
         <v>1241</v>
       </c>
       <c r="F197" s="1" t="s">
-        <v>1846</v>
+        <v>1867</v>
       </c>
       <c r="G197" s="1" t="s">
-        <v>1847</v>
+        <v>1868</v>
       </c>
       <c r="H197" s="1" t="s">
         <v>1243</v>
       </c>
       <c r="I197" s="1" t="s">
-        <v>1848</v>
+        <v>1869</v>
       </c>
       <c r="J197" s="1" t="s">
-        <v>1771</v>
+        <v>1792</v>
       </c>
       <c r="K197" s="1" t="s">
         <v>44</v>
@@ -57661,7 +57762,7 @@
         <v>43</v>
       </c>
       <c r="M197" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="198">
@@ -57698,7 +57799,7 @@
         <v>1256</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>1849</v>
+        <v>1870</v>
       </c>
       <c r="G199" s="1" t="s">
         <v>1257</v>
@@ -57710,7 +57811,7 @@
         <v>1259</v>
       </c>
       <c r="J199" s="1" t="s">
-        <v>1850</v>
+        <v>1871</v>
       </c>
       <c r="K199" s="1" t="s">
         <v>25</v>
@@ -57719,7 +57820,7 @@
         <v>43</v>
       </c>
       <c r="M199" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="200">
@@ -57773,19 +57874,19 @@
         <v>1273</v>
       </c>
       <c r="F202" s="1" t="s">
-        <v>1851</v>
+        <v>1872</v>
       </c>
       <c r="G202" s="1" t="s">
-        <v>1852</v>
+        <v>1873</v>
       </c>
       <c r="H202" s="1" t="s">
         <v>1275</v>
       </c>
       <c r="I202" s="1" t="s">
-        <v>1853</v>
+        <v>1874</v>
       </c>
       <c r="J202" s="1" t="s">
-        <v>1854</v>
+        <v>1875</v>
       </c>
       <c r="K202" s="1" t="s">
         <v>25</v>
@@ -57794,7 +57895,7 @@
         <v>205</v>
       </c>
       <c r="M202" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="203">
@@ -57829,19 +57930,19 @@
         <v>2624.0</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>1855</v>
+        <v>1876</v>
       </c>
       <c r="G204" s="1" t="s">
         <v>1288</v>
       </c>
       <c r="H204" s="1" t="s">
-        <v>1856</v>
+        <v>1877</v>
       </c>
       <c r="I204" s="1" t="s">
         <v>1290</v>
       </c>
       <c r="J204" s="1" t="s">
-        <v>1857</v>
+        <v>1878</v>
       </c>
       <c r="K204" s="1" t="s">
         <v>44</v>
@@ -57850,7 +57951,7 @@
         <v>26</v>
       </c>
       <c r="M204" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="205">
@@ -57869,7 +57970,7 @@
       <c r="M205" s="7"/>
     </row>
     <row r="206">
-      <c r="A206" s="26" t="s">
+      <c r="A206" s="27" t="s">
         <v>1297</v>
       </c>
       <c r="B206" s="1" t="s">
@@ -57885,17 +57986,17 @@
         <v>1301</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>1858</v>
+        <v>1879</v>
       </c>
       <c r="G206" s="1" t="s">
         <v>1302</v>
       </c>
       <c r="H206" s="7"/>
       <c r="I206" s="1" t="s">
-        <v>1859</v>
+        <v>1880</v>
       </c>
       <c r="J206" s="1" t="s">
-        <v>1660</v>
+        <v>1681</v>
       </c>
       <c r="K206" s="1" t="s">
         <v>25</v>
@@ -57904,7 +58005,7 @@
         <v>26</v>
       </c>
       <c r="M206" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="207">
@@ -57937,15 +58038,15 @@
         <v>1314</v>
       </c>
       <c r="F208" s="1" t="s">
-        <v>1860</v>
+        <v>1881</v>
       </c>
       <c r="G208" s="1" t="s">
-        <v>1861</v>
+        <v>1882</v>
       </c>
       <c r="H208" s="7"/>
       <c r="I208" s="7"/>
       <c r="J208" s="1" t="s">
-        <v>1862</v>
+        <v>1883</v>
       </c>
       <c r="K208" s="1" t="s">
         <v>25</v>
@@ -57954,7 +58055,7 @@
         <v>43</v>
       </c>
       <c r="M208" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="209">
@@ -57989,7 +58090,7 @@
         <v>12049.0</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>1863</v>
+        <v>1884</v>
       </c>
       <c r="G210" s="1" t="s">
         <v>1329</v>
@@ -57998,10 +58099,10 @@
         <v>1330</v>
       </c>
       <c r="I210" s="1" t="s">
-        <v>1864</v>
+        <v>1885</v>
       </c>
       <c r="J210" s="1" t="s">
-        <v>1865</v>
+        <v>1886</v>
       </c>
       <c r="K210" s="1" t="s">
         <v>25</v>
@@ -58010,7 +58111,7 @@
         <v>43</v>
       </c>
       <c r="M210" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="211">
@@ -58033,7 +58134,7 @@
         <v>1339</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>1866</v>
+        <v>1887</v>
       </c>
       <c r="C212" s="4" t="s">
         <v>1341</v>
@@ -58045,19 +58146,19 @@
         <v>1343</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>1867</v>
+        <v>1888</v>
       </c>
       <c r="G212" s="1" t="s">
         <v>1344</v>
       </c>
       <c r="H212" s="1" t="s">
-        <v>1868</v>
+        <v>1889</v>
       </c>
       <c r="I212" s="1" t="s">
-        <v>1869</v>
+        <v>1890</v>
       </c>
       <c r="J212" s="18" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
       <c r="K212" s="1" t="s">
         <v>25</v>
@@ -58066,7 +58167,7 @@
         <v>26</v>
       </c>
       <c r="M212" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="213">
@@ -58120,7 +58221,7 @@
         <v>1359</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>1870</v>
+        <v>1891</v>
       </c>
       <c r="G215" s="1" t="s">
         <v>1360</v>
@@ -58132,7 +58233,7 @@
         <v>1362</v>
       </c>
       <c r="J215" s="1" t="s">
-        <v>1679</v>
+        <v>1700</v>
       </c>
       <c r="K215" s="1" t="s">
         <v>25</v>
@@ -58141,7 +58242,7 @@
         <v>43</v>
       </c>
       <c r="M215" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="216">
@@ -58229,7 +58330,7 @@
         <v>1376</v>
       </c>
       <c r="F220" s="1" t="s">
-        <v>1871</v>
+        <v>1892</v>
       </c>
       <c r="G220" s="1" t="s">
         <v>1377</v>
@@ -58241,7 +58342,7 @@
         <v>1379</v>
       </c>
       <c r="J220" s="1" t="s">
-        <v>1733</v>
+        <v>1754</v>
       </c>
       <c r="K220" s="1" t="s">
         <v>25</v>
@@ -58250,7 +58351,7 @@
         <v>205</v>
       </c>
       <c r="M220" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="221">
@@ -58287,7 +58388,7 @@
         <v>57147.0</v>
       </c>
       <c r="F222" s="1" t="s">
-        <v>1872</v>
+        <v>1893</v>
       </c>
       <c r="G222" s="1" t="s">
         <v>1391</v>
@@ -58299,7 +58400,7 @@
         <v>1393</v>
       </c>
       <c r="J222" s="1" t="s">
-        <v>1733</v>
+        <v>1754</v>
       </c>
       <c r="K222" s="1" t="s">
         <v>44</v>
@@ -58308,7 +58409,7 @@
         <v>43</v>
       </c>
       <c r="M222" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="223">
@@ -58337,23 +58438,23 @@
         <v>1401</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>1873</v>
+        <v>1894</v>
       </c>
       <c r="E224" s="1" t="s">
         <v>1403</v>
       </c>
       <c r="F224" s="1" t="s">
-        <v>1874</v>
+        <v>1895</v>
       </c>
       <c r="G224" s="1" t="s">
         <v>417</v>
       </c>
       <c r="H224" s="7"/>
       <c r="I224" s="1" t="s">
-        <v>1875</v>
+        <v>1896</v>
       </c>
       <c r="J224" s="1" t="s">
-        <v>1876</v>
+        <v>1897</v>
       </c>
       <c r="K224" s="1" t="s">
         <v>44</v>
@@ -58362,7 +58463,7 @@
         <v>205</v>
       </c>
       <c r="M224" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="225">
@@ -58399,7 +58500,7 @@
       <c r="H226" s="7"/>
       <c r="I226" s="7"/>
       <c r="J226" s="1" t="s">
-        <v>1877</v>
+        <v>1898</v>
       </c>
       <c r="K226" s="1" t="s">
         <v>44</v>
@@ -58408,7 +58509,7 @@
         <v>205</v>
       </c>
       <c r="M226" s="1" t="s">
-        <v>1580</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="227">
@@ -58511,7 +58612,7 @@
     </row>
     <row r="233">
       <c r="A233" s="1" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
       <c r="B233" s="7"/>
       <c r="C233" s="7"/>
@@ -58528,7 +58629,7 @@
     </row>
     <row r="234">
       <c r="A234" s="1" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="B234" s="7"/>
       <c r="C234" s="7"/>
@@ -58560,7 +58661,7 @@
     </row>
     <row r="236">
       <c r="A236" s="1" t="s">
-        <v>1494</v>
+        <v>1497</v>
       </c>
       <c r="B236" s="7"/>
       <c r="C236" s="7"/>
@@ -58577,7 +58678,7 @@
     </row>
     <row r="237">
       <c r="A237" s="1" t="s">
-        <v>1507</v>
+        <v>1510</v>
       </c>
       <c r="B237" s="7"/>
       <c r="C237" s="7"/>
@@ -58594,7 +58695,7 @@
     </row>
     <row r="238">
       <c r="A238" s="1" t="s">
-        <v>1520</v>
+        <v>1523</v>
       </c>
       <c r="B238" s="7"/>
       <c r="C238" s="7"/>
@@ -58611,7 +58712,7 @@
     </row>
     <row r="239">
       <c r="A239" s="1" t="s">
-        <v>1533</v>
+        <v>1536</v>
       </c>
       <c r="B239" s="7"/>
       <c r="C239" s="7"/>
@@ -58628,7 +58729,7 @@
     </row>
     <row r="240">
       <c r="A240" s="1" t="s">
-        <v>1548</v>
+        <v>1551</v>
       </c>
       <c r="B240" s="7"/>
       <c r="C240" s="7"/>

</xml_diff>